<commit_message>
Problem 101, 104, 107, 108 & 110
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A04E1A7-27F9-4950-9C7E-4322B98BBA9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2FDCE5-BCC7-4918-8FEB-9A0F1620777A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,21 @@
   </si>
   <si>
     <t>Palindromic Substrings</t>
+  </si>
+  <si>
+    <t>Symmetric Tree</t>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>Binary Tree Level Order Traversal II</t>
+  </si>
+  <si>
+    <t>Convert Sorted Array to Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Balanced Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -726,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,6 +1165,56 @@
       <c r="C39" s="17"/>
       <c r="D39" s="12"/>
     </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="14">
+        <v>101</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="16"/>
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="14">
+        <v>104</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="14">
+        <v>107</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="16"/>
+      <c r="D42" s="12"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="14">
+        <v>108</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="16"/>
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="14">
+        <v>110</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="16"/>
+      <c r="D44" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Problem 6 & 8
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2FDCE5-BCC7-4918-8FEB-9A0F1620777A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D277518-2F87-4C6D-A7B2-E678FC20AD3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>Balanced Binary Tree</t>
+  </si>
+  <si>
+    <t>ZigZag Conversion</t>
+  </si>
+  <si>
+    <t>String to Integer</t>
   </si>
 </sst>
 </file>
@@ -741,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1215,6 +1221,26 @@
       <c r="C44" s="16"/>
       <c r="D44" s="12"/>
     </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="14">
+        <v>6</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="17"/>
+      <c r="D45" s="13"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="14">
+        <v>8</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="17"/>
+      <c r="D46" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Problem 11, 12 and 51
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D277518-2F87-4C6D-A7B2-E678FC20AD3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85507E3C-EF90-48FE-98E9-3CA91948BF90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>String to Integer</t>
+  </si>
+  <si>
+    <t>N-Queens</t>
+  </si>
+  <si>
+    <t>Integer to Roman</t>
+  </si>
+  <si>
+    <t>Container With Most Water</t>
   </si>
 </sst>
 </file>
@@ -747,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1241,6 +1250,36 @@
       <c r="C46" s="17"/>
       <c r="D46" s="12"/>
     </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="14">
+        <v>51</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="18"/>
+      <c r="D47" s="13"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="14">
+        <v>12</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="17"/>
+      <c r="D48" s="12"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="14">
+        <v>11</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="17"/>
+      <c r="D49" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Problem 16, 17 & 18
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85507E3C-EF90-48FE-98E9-3CA91948BF90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13856D32-68BE-4780-A1DD-153E1E2F4337}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>Container With Most Water</t>
+  </si>
+  <si>
+    <t>Letter Combinations of a Phone Number</t>
+  </si>
+  <si>
+    <t>4Sum</t>
+  </si>
+  <si>
+    <t>3Sum Closest</t>
   </si>
 </sst>
 </file>
@@ -756,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1280,6 +1289,36 @@
       <c r="C49" s="17"/>
       <c r="D49" s="12"/>
     </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="14">
+        <v>16</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="17"/>
+      <c r="D50" s="12"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="14">
+        <v>17</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="17"/>
+      <c r="D51" s="11"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="14">
+        <v>18</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="17"/>
+      <c r="D52" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Problem 19, 22, 24, 29 & 31
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13856D32-68BE-4780-A1DD-153E1E2F4337}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73136FED-DBB6-4F03-838A-AA9B4AC5F5C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>3Sum Closest</t>
+  </si>
+  <si>
+    <t>Remove Nth Node From End of List</t>
+  </si>
+  <si>
+    <t>Swap Nodes in Pairs</t>
+  </si>
+  <si>
+    <t>Divide Two Integers</t>
+  </si>
+  <si>
+    <t>Next Permutation</t>
   </si>
 </sst>
 </file>
@@ -765,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1319,6 +1331,46 @@
       <c r="C52" s="17"/>
       <c r="D52" s="12"/>
     </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="14">
+        <v>19</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="17"/>
+      <c r="D53" s="11"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="14">
+        <v>25</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="17"/>
+      <c r="D54" s="12"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="14">
+        <v>29</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" s="17"/>
+      <c r="D55" s="13"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="14">
+        <v>31</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="17"/>
+      <c r="D56" s="13"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Problem 111, 112 & 118
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DD17FF-2C47-42A9-8C99-4CDF4B845EC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68F93FE-552F-4615-86EA-11F6EDE76A16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t>Minimum Number of Days to Eat N Oranges</t>
+  </si>
+  <si>
+    <t>Minimum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>Path Sum</t>
+  </si>
+  <si>
+    <t>Pascal's Triangle</t>
   </si>
 </sst>
 </file>
@@ -795,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1439,6 +1448,36 @@
       <c r="C61" s="17"/>
       <c r="D61" s="12"/>
     </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="14">
+        <v>111</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C62" s="15"/>
+      <c r="D62" s="11"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="14">
+        <v>112</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C63" s="15"/>
+      <c r="D63" s="11"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="14">
+        <v>118</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64" s="15"/>
+      <c r="D64" s="12"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D57">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Problem 119, 121, 122, 125, 136 & 141
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68F93FE-552F-4615-86EA-11F6EDE76A16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BE17A9-7FBD-459C-AD2B-47A4D47839FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -235,6 +235,24 @@
   </si>
   <si>
     <t>Pascal's Triangle</t>
+  </si>
+  <si>
+    <t>Pascal's Triangle - II</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock - II</t>
+  </si>
+  <si>
+    <t>Valid Palindrome</t>
+  </si>
+  <si>
+    <t>Single Number</t>
+  </si>
+  <si>
+    <t>Linked List Cycle</t>
   </si>
 </sst>
 </file>
@@ -804,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1478,6 +1496,66 @@
       <c r="C64" s="15"/>
       <c r="D64" s="12"/>
     </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="14">
+        <v>119</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" s="15"/>
+      <c r="D65" s="12"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="14">
+        <v>121</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C66" s="15"/>
+      <c r="D66" s="11"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="14">
+        <v>122</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C67" s="15"/>
+      <c r="D67" s="11"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="14">
+        <v>125</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" s="15"/>
+      <c r="D68" s="11"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="14">
+        <v>136</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C69" s="15"/>
+      <c r="D69" s="11"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="14">
+        <v>141</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C70" s="15"/>
+      <c r="D70" s="11"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D57">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Problem 33 & 36
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BE17A9-7FBD-459C-AD2B-47A4D47839FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B49081-FAF6-49D0-B08D-E57E81573BF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>Linked List Cycle</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Valid Sudoku</t>
   </si>
 </sst>
 </file>
@@ -334,7 +340,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -432,6 +438,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -439,7 +460,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -503,6 +524,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -822,16 +846,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.5546875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="46.109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="47.77734375" style="14" customWidth="1"/>
     <col min="3" max="3" width="23.77734375" style="18" customWidth="1"/>
     <col min="4" max="4" width="24.21875" style="14" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
@@ -1138,426 +1162,446 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="14">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="12"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="14">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="12"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="14">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="15"/>
-      <c r="D31" s="13"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="14">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="13"/>
+        <v>77</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="12"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="14">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C33" s="22"/>
-      <c r="D33" s="11"/>
+      <c r="D33" s="13"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="14">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="C34" s="17"/>
+      <c r="D34" s="13"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="14">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="14">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C36" s="15"/>
       <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="14">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C37" s="15"/>
       <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="14">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C38" s="15"/>
       <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="14">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C40" s="15"/>
-      <c r="D40" s="12"/>
+      <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="14">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C41" s="15"/>
-      <c r="D41" s="12"/>
+      <c r="D41" s="11"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="14">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C42" s="15"/>
-      <c r="D42" s="11"/>
+      <c r="D42" s="12"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C43" s="15"/>
-      <c r="D43" s="11"/>
+      <c r="D43" s="12"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="14">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C44" s="15"/>
-      <c r="D44" s="12"/>
+      <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="14">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="14">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C46" s="15"/>
       <c r="D46" s="12"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="14">
-        <v>152</v>
+        <v>108</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="12"/>
+        <v>48</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="14">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C48" s="15"/>
       <c r="D48" s="12"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="14">
-        <v>206</v>
+        <v>111</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="C49" s="15"/>
       <c r="D49" s="11"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="14">
-        <v>215</v>
+        <v>112</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C50" s="16"/>
-      <c r="D50" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="11"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
-        <v>234</v>
+        <v>118</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C51" s="21"/>
+        <v>69</v>
+      </c>
+      <c r="C51" s="15"/>
       <c r="D51" s="12"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="14">
-        <v>238</v>
+        <v>119</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C52" s="16"/>
-      <c r="D52" s="13"/>
+        <v>70</v>
+      </c>
+      <c r="C52" s="15"/>
+      <c r="D52" s="12"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="14">
-        <v>300</v>
+        <v>121</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53" s="16"/>
-      <c r="D53" s="13"/>
+        <v>71</v>
+      </c>
+      <c r="C53" s="15"/>
+      <c r="D53" s="11"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
-        <v>322</v>
+        <v>122</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C54" s="16"/>
-      <c r="D54" s="13"/>
+        <v>72</v>
+      </c>
+      <c r="C54" s="15"/>
+      <c r="D54" s="11"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="14">
-        <v>373</v>
+        <v>125</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C55" s="16"/>
-      <c r="D55" s="13"/>
+        <v>73</v>
+      </c>
+      <c r="C55" s="15"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="14">
-        <v>394</v>
+        <v>136</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C56" s="16"/>
-      <c r="D56" s="12"/>
+        <v>74</v>
+      </c>
+      <c r="C56" s="15"/>
+      <c r="D56" s="11"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="14">
-        <v>647</v>
+        <v>141</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C57" s="16"/>
-      <c r="D57" s="12"/>
+        <v>75</v>
+      </c>
+      <c r="C57" s="15"/>
+      <c r="D57" s="11"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="14">
-        <v>1550</v>
+        <v>152</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="11"/>
+        <v>34</v>
+      </c>
+      <c r="C58" s="16"/>
+      <c r="D58" s="12"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="14">
-        <v>1551</v>
+        <v>160</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C59" s="16"/>
-      <c r="D59" s="11"/>
+        <v>35</v>
+      </c>
+      <c r="C59" s="15"/>
+      <c r="D59" s="12"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="14">
-        <v>1552</v>
+        <v>206</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C60" s="16"/>
-      <c r="D60" s="13"/>
+        <v>36</v>
+      </c>
+      <c r="C60" s="15"/>
+      <c r="D60" s="11"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="14">
-        <v>1553</v>
+        <v>215</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C61" s="17"/>
+        <v>37</v>
+      </c>
+      <c r="C61" s="16"/>
       <c r="D61" s="12"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="14">
-        <v>111</v>
+        <v>234</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="11"/>
+        <v>38</v>
+      </c>
+      <c r="C62" s="21"/>
+      <c r="D62" s="12"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="14">
-        <v>112</v>
+        <v>238</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C63" s="15"/>
-      <c r="D63" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="C63" s="16"/>
+      <c r="D63" s="13"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="14">
-        <v>118</v>
+        <v>300</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="12"/>
+        <v>40</v>
+      </c>
+      <c r="C64" s="16"/>
+      <c r="D64" s="13"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
-        <v>119</v>
+        <v>322</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C65" s="15"/>
-      <c r="D65" s="12"/>
+        <v>41</v>
+      </c>
+      <c r="C65" s="16"/>
+      <c r="D65" s="13"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="14">
-        <v>121</v>
+        <v>373</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C66" s="15"/>
-      <c r="D66" s="11"/>
+        <v>42</v>
+      </c>
+      <c r="C66" s="16"/>
+      <c r="D66" s="13"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="14">
-        <v>122</v>
+        <v>394</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C67" s="15"/>
-      <c r="D67" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="C67" s="16"/>
+      <c r="D67" s="12"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
-        <v>125</v>
+        <v>647</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C68" s="15"/>
-      <c r="D68" s="11"/>
+        <v>44</v>
+      </c>
+      <c r="C68" s="16"/>
+      <c r="D68" s="12"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="14">
-        <v>136</v>
+        <v>1550</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C69" s="15"/>
       <c r="D69" s="11"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="14">
-        <v>141</v>
+        <v>1551</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C70" s="15"/>
+        <v>64</v>
+      </c>
+      <c r="C70" s="16"/>
       <c r="D70" s="11"/>
     </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="14">
+        <v>1552</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C71" s="23"/>
+      <c r="D71" s="13"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="14">
+        <v>1553</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C72" s="17"/>
+      <c r="D72" s="12"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D57">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D72">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Problem 40 & 43
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813558CC-4AF0-4854-960E-DE754337CC10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AD8E82-B444-4A61-AFD4-E773A048CFA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>Combination Sum</t>
+  </si>
+  <si>
+    <t>Multiply Strings</t>
   </si>
 </sst>
 </file>
@@ -852,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1224,7 +1227,7 @@
         <v>78</v>
       </c>
       <c r="C34" s="16"/>
-      <c r="D34" s="12"/>
+      <c r="D34" s="13"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="14">
@@ -1615,6 +1618,26 @@
       </c>
       <c r="C73" s="24"/>
       <c r="D73" s="12"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="14">
+        <v>40</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74" s="16"/>
+      <c r="D74" s="13"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="14">
+        <v>43</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75" s="16"/>
+      <c r="D75" s="13"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D73">

</xml_diff>

<commit_message>
Biweekly Contest 33 Problem 5479
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AD8E82-B444-4A61-AFD4-E773A048CFA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A569499E-474B-47EF-95A1-F15DB98CB19C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
   <si>
     <t>Name</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>Multiply Strings</t>
+  </si>
+  <si>
+    <t>Thousand Separator</t>
   </si>
 </sst>
 </file>
@@ -855,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1639,6 +1642,16 @@
       <c r="C75" s="16"/>
       <c r="D75" s="13"/>
     </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="14">
+        <v>5479</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C76" s="15"/>
+      <c r="D76" s="11"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D73">
     <sortCondition ref="A40"/>

</xml_diff>

<commit_message>
Biweekly Contest 33 Problems 1557 & 1558
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A569499E-474B-47EF-95A1-F15DB98CB19C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB027353-0359-4C65-8AC3-DFC0AD5732A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>Thousand Separator</t>
+  </si>
+  <si>
+    <t>Minimum Number of Vertices to Reach All Nodes</t>
+  </si>
+  <si>
+    <t>Minimum Number of Function Calls to Make Target Array</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -536,9 +542,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -858,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1234,417 +1237,417 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="14">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="17"/>
+        <v>78</v>
+      </c>
+      <c r="C35" s="16"/>
       <c r="D35" s="13"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="14">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="11"/>
+        <v>79</v>
+      </c>
+      <c r="C36" s="16"/>
+      <c r="D36" s="13"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="14">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="C37" s="17"/>
+      <c r="D37" s="13"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="14">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C38" s="15"/>
       <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="14">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C40" s="15"/>
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="14">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="11"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="14">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C42" s="15"/>
       <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C43" s="15"/>
-      <c r="D43" s="12"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="14">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C44" s="15"/>
-      <c r="D44" s="12"/>
+      <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="14">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C45" s="15"/>
-      <c r="D45" s="11"/>
+      <c r="D45" s="12"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="14">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C46" s="15"/>
-      <c r="D46" s="11"/>
+      <c r="D46" s="12"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="14">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="D47" s="12"/>
+      <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="14">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C48" s="15"/>
       <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="14">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C49" s="15"/>
       <c r="D49" s="12"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="14">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C50" s="15"/>
       <c r="D50" s="11"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="D51" s="11"/>
+      <c r="D51" s="12"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="14">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C52" s="15"/>
-      <c r="D52" s="12"/>
+      <c r="D52" s="11"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="14">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="D53" s="12"/>
+      <c r="D53" s="11"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C54" s="15"/>
-      <c r="D54" s="11"/>
+      <c r="D54" s="12"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="14">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="D55" s="11"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="14">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C56" s="15"/>
       <c r="D56" s="11"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="14">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C57" s="15"/>
       <c r="D57" s="11"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="14">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C58" s="15"/>
       <c r="D58" s="11"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="14">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="16"/>
-      <c r="D59" s="12"/>
+        <v>74</v>
+      </c>
+      <c r="C59" s="15"/>
+      <c r="D59" s="11"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="14">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="C60" s="15"/>
-      <c r="D60" s="12"/>
+      <c r="D60" s="11"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="14">
-        <v>206</v>
+        <v>152</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C61" s="15"/>
-      <c r="D61" s="11"/>
+        <v>34</v>
+      </c>
+      <c r="C61" s="16"/>
+      <c r="D61" s="12"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="14">
-        <v>215</v>
+        <v>160</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C62" s="16"/>
+        <v>35</v>
+      </c>
+      <c r="C62" s="15"/>
       <c r="D62" s="12"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="14">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C63" s="21"/>
-      <c r="D63" s="12"/>
+        <v>36</v>
+      </c>
+      <c r="C63" s="15"/>
+      <c r="D63" s="11"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="14">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C64" s="16"/>
-      <c r="D64" s="13"/>
+      <c r="D64" s="12"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
-        <v>300</v>
+        <v>234</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C65" s="16"/>
-      <c r="D65" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="C65" s="21"/>
+      <c r="D65" s="12"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="14">
-        <v>322</v>
+        <v>238</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C66" s="16"/>
       <c r="D66" s="13"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="14">
-        <v>373</v>
+        <v>300</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C67" s="16"/>
       <c r="D67" s="13"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
-        <v>394</v>
+        <v>322</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C68" s="16"/>
-      <c r="D68" s="12"/>
+      <c r="D68" s="13"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="14">
-        <v>647</v>
+        <v>373</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C69" s="16"/>
-      <c r="D69" s="12"/>
+      <c r="D69" s="13"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="14">
-        <v>1550</v>
+        <v>394</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="C70" s="16"/>
+      <c r="D70" s="12"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="14">
-        <v>1551</v>
+        <v>647</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="C71" s="23"/>
-      <c r="D71" s="11"/>
+      <c r="D71" s="12"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="14">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C72" s="16"/>
-      <c r="D72" s="13"/>
+        <v>63</v>
+      </c>
+      <c r="C72" s="15"/>
+      <c r="D72" s="11"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="14">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C73" s="24"/>
-      <c r="D73" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="C73" s="23"/>
+      <c r="D73" s="11"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="14">
-        <v>40</v>
+        <v>1552</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C74" s="16"/>
       <c r="D74" s="13"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="14">
-        <v>43</v>
+        <v>1553</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C75" s="16"/>
-      <c r="D75" s="13"/>
+        <v>66</v>
+      </c>
+      <c r="C75" s="17"/>
+      <c r="D75" s="12"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="14">
-        <v>5479</v>
+        <v>1556</v>
       </c>
       <c r="B76" s="14" t="s">
         <v>80</v>
@@ -1652,9 +1655,29 @@
       <c r="C76" s="15"/>
       <c r="D76" s="11"/>
     </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="14">
+        <v>1557</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77" s="16"/>
+      <c r="D77" s="12"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="14">
+        <v>1558</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78" s="16"/>
+      <c r="D78" s="13"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D73">
-    <sortCondition ref="A40"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D79">
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Problem 155, 167 & 168
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB027353-0359-4C65-8AC3-DFC0AD5732A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F311EC8C-2778-4068-8214-B458D46E7BCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -274,6 +274,15 @@
   </si>
   <si>
     <t>Minimum Number of Function Calls to Make Target Array</t>
+  </si>
+  <si>
+    <t>Min Stack</t>
+  </si>
+  <si>
+    <t>Two Sum II Input array is sorted</t>
+  </si>
+  <si>
+    <t>Excel Sheet Column Title</t>
   </si>
 </sst>
 </file>
@@ -861,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1507,177 +1516,207 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="14">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="C62" s="15"/>
-      <c r="D62" s="12"/>
+      <c r="D62" s="11"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="14">
-        <v>206</v>
+        <v>160</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C63" s="15"/>
-      <c r="D63" s="11"/>
+      <c r="D63" s="12"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="14">
-        <v>215</v>
+        <v>167</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C64" s="16"/>
-      <c r="D64" s="12"/>
+        <v>84</v>
+      </c>
+      <c r="C64" s="15"/>
+      <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
-        <v>234</v>
+        <v>168</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C65" s="21"/>
+        <v>85</v>
+      </c>
+      <c r="C65" s="15"/>
       <c r="D65" s="12"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="14">
-        <v>238</v>
+        <v>206</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C66" s="16"/>
-      <c r="D66" s="13"/>
+        <v>36</v>
+      </c>
+      <c r="C66" s="15"/>
+      <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="14">
-        <v>300</v>
+        <v>215</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C67" s="16"/>
-      <c r="D67" s="13"/>
+      <c r="D67" s="12"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
-        <v>322</v>
+        <v>234</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C68" s="16"/>
-      <c r="D68" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="C68" s="21"/>
+      <c r="D68" s="12"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="14">
-        <v>373</v>
+        <v>238</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C69" s="16"/>
       <c r="D69" s="13"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="14">
-        <v>394</v>
+        <v>300</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C70" s="16"/>
-      <c r="D70" s="12"/>
+      <c r="D70" s="13"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="14">
-        <v>647</v>
+        <v>322</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C71" s="23"/>
-      <c r="D71" s="12"/>
+      <c r="D71" s="13"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="14">
-        <v>1550</v>
+        <v>373</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="11"/>
+        <v>42</v>
+      </c>
+      <c r="C72" s="16"/>
+      <c r="D72" s="13"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="14">
-        <v>1551</v>
+        <v>394</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C73" s="23"/>
-      <c r="D73" s="11"/>
+      <c r="D73" s="12"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="14">
-        <v>1552</v>
+        <v>647</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="C74" s="16"/>
-      <c r="D74" s="13"/>
+      <c r="D74" s="12"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="14">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C75" s="17"/>
-      <c r="D75" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="C75" s="15"/>
+      <c r="D75" s="11"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="14">
-        <v>1556</v>
+        <v>1551</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C76" s="15"/>
+        <v>64</v>
+      </c>
+      <c r="C76" s="16"/>
       <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="14">
-        <v>1557</v>
+        <v>1552</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C77" s="16"/>
-      <c r="D77" s="12"/>
+      <c r="D77" s="13"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="14">
+        <v>1553</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C78" s="17"/>
+      <c r="D78" s="12"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="14">
+        <v>1556</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C79" s="15"/>
+      <c r="D79" s="11"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="14">
+        <v>1557</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" s="16"/>
+      <c r="D80" s="12"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="14">
         <v>1558</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B81" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C78" s="16"/>
-      <c r="D78" s="13"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="13"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D79">
-    <sortCondition ref="A1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D81">
+    <sortCondition ref="A55"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Problem 46 & 47
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C4F2BF-5DCB-47BA-A7A8-EA9F5E7A328C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35DFB6C-9B3E-40B4-9971-A3EAE79FA446}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>Majority Element</t>
+  </si>
+  <si>
+    <t>Permutations</t>
+  </si>
+  <si>
+    <t>Permutations II</t>
   </si>
 </sst>
 </file>
@@ -549,13 +555,13 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -873,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1234,7 +1240,7 @@
       <c r="B33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="22"/>
+      <c r="C33" s="21"/>
       <c r="D33" s="13"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1269,467 +1275,487 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="14">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="13"/>
+        <v>87</v>
+      </c>
+      <c r="C37" s="16"/>
+      <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="14">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="15"/>
+        <v>88</v>
+      </c>
+      <c r="C38" s="16"/>
       <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="14">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="15"/>
-      <c r="D39" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="C39" s="17"/>
+      <c r="D39" s="13"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C40" s="15"/>
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="14">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="11"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="14">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C42" s="15"/>
       <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C43" s="15"/>
       <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="14">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C44" s="15"/>
       <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="14">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C45" s="15"/>
-      <c r="D45" s="12"/>
+      <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="14">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C46" s="15"/>
-      <c r="D46" s="12"/>
+      <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="14">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="D47" s="11"/>
+      <c r="D47" s="12"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="14">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C48" s="15"/>
-      <c r="D48" s="11"/>
+      <c r="D48" s="12"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="14">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C49" s="15"/>
-      <c r="D49" s="12"/>
+      <c r="D49" s="11"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="14">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C50" s="15"/>
       <c r="D50" s="11"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="12"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="14">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C52" s="15"/>
       <c r="D52" s="11"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="14">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="D53" s="11"/>
+      <c r="D53" s="12"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C54" s="15"/>
-      <c r="D54" s="12"/>
+      <c r="D54" s="11"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="14">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="D55" s="12"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="14">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C56" s="15"/>
-      <c r="D56" s="11"/>
+      <c r="D56" s="12"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="14">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C57" s="15"/>
-      <c r="D57" s="11"/>
+      <c r="D57" s="12"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="14">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C58" s="15"/>
       <c r="D58" s="11"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="14">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="11"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="14">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="11"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="14">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C61" s="16"/>
-      <c r="D61" s="12"/>
+        <v>74</v>
+      </c>
+      <c r="C61" s="15"/>
+      <c r="D61" s="11"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="14">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="11"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="14">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C63" s="15"/>
+        <v>34</v>
+      </c>
+      <c r="C63" s="16"/>
       <c r="D63" s="12"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="14">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="12"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="14">
-        <v>206</v>
+        <v>167</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="14">
-        <v>215</v>
+        <v>168</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C67" s="16"/>
+        <v>85</v>
+      </c>
+      <c r="C67" s="15"/>
       <c r="D67" s="12"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
-        <v>234</v>
+        <v>169</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C68" s="21"/>
-      <c r="D68" s="12"/>
+        <v>86</v>
+      </c>
+      <c r="C68" s="15"/>
+      <c r="D68" s="11"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="14">
-        <v>238</v>
+        <v>206</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C69" s="16"/>
-      <c r="D69" s="13"/>
+        <v>36</v>
+      </c>
+      <c r="C69" s="15"/>
+      <c r="D69" s="11"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="14">
-        <v>300</v>
+        <v>215</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C70" s="16"/>
-      <c r="D70" s="13"/>
+      <c r="D70" s="12"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="14">
-        <v>322</v>
+        <v>234</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C71" s="23"/>
-      <c r="D71" s="13"/>
+      <c r="D71" s="12"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="14">
-        <v>373</v>
+        <v>238</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C72" s="16"/>
       <c r="D72" s="13"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="14">
-        <v>394</v>
+        <v>300</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C73" s="23"/>
-      <c r="D73" s="12"/>
+        <v>40</v>
+      </c>
+      <c r="C73" s="22"/>
+      <c r="D73" s="13"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="14">
-        <v>647</v>
+        <v>322</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C74" s="16"/>
-      <c r="D74" s="12"/>
+      <c r="D74" s="13"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="14">
-        <v>1550</v>
+        <v>373</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C75" s="15"/>
-      <c r="D75" s="11"/>
+        <v>42</v>
+      </c>
+      <c r="C75" s="16"/>
+      <c r="D75" s="13"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="14">
-        <v>1551</v>
+        <v>394</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C76" s="16"/>
-      <c r="D76" s="11"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="14">
-        <v>1552</v>
+        <v>647</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="C77" s="16"/>
-      <c r="D77" s="13"/>
+      <c r="D77" s="12"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="14">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C78" s="17"/>
-      <c r="D78" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="C78" s="15"/>
+      <c r="D78" s="11"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="14">
-        <v>1556</v>
+        <v>1551</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C79" s="15"/>
+        <v>64</v>
+      </c>
+      <c r="C79" s="16"/>
       <c r="D79" s="11"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="14">
-        <v>1557</v>
+        <v>1552</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C80" s="16"/>
-      <c r="D80" s="12"/>
+      <c r="D80" s="13"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="14">
-        <v>1558</v>
+        <v>1553</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C81" s="16"/>
-      <c r="D81" s="13"/>
+        <v>66</v>
+      </c>
+      <c r="C81" s="17"/>
+      <c r="D81" s="12"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="14">
-        <v>169</v>
+        <v>1556</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C82" s="15"/>
       <c r="D82" s="11"/>
     </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="14">
+        <v>1557</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C83" s="16"/>
+      <c r="D83" s="12"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="14">
+        <v>1558</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C84" s="16"/>
+      <c r="D84" s="13"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D81">
-    <sortCondition ref="A55"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D84">
+    <sortCondition ref="A64"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Problem 48 & 49
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35DFB6C-9B3E-40B4-9971-A3EAE79FA446}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A83E1EB-F1C6-43F8-9ACC-014570BBAF95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -292,6 +292,12 @@
   </si>
   <si>
     <t>Permutations II</t>
+  </si>
+  <si>
+    <t>Rotate Image</t>
+  </si>
+  <si>
+    <t>Group Anagrams</t>
   </si>
 </sst>
 </file>
@@ -558,10 +564,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -879,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J84"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1295,467 +1301,487 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="14">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="13"/>
+        <v>89</v>
+      </c>
+      <c r="C39" s="16"/>
+      <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="15"/>
+        <v>90</v>
+      </c>
+      <c r="C40" s="16"/>
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="14">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="C41" s="17"/>
+      <c r="D41" s="13"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="14">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C42" s="15"/>
       <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C43" s="15"/>
       <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="14">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C44" s="15"/>
       <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="14">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="14">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C46" s="15"/>
       <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="14">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="D47" s="12"/>
+      <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="14">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C48" s="15"/>
-      <c r="D48" s="12"/>
+      <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="14">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C49" s="15"/>
-      <c r="D49" s="11"/>
+      <c r="D49" s="12"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="14">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C50" s="15"/>
-      <c r="D50" s="11"/>
+      <c r="D50" s="12"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="D51" s="12"/>
+      <c r="D51" s="11"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="14">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C52" s="15"/>
       <c r="D52" s="11"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="14">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C53" s="15"/>
       <c r="D53" s="12"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="11"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="14">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="D55" s="11"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="14">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C56" s="15"/>
-      <c r="D56" s="12"/>
+      <c r="D56" s="11"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="14">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C57" s="15"/>
-      <c r="D57" s="12"/>
+      <c r="D57" s="11"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="14">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C58" s="15"/>
-      <c r="D58" s="11"/>
+      <c r="D58" s="12"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="14">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C59" s="15"/>
-      <c r="D59" s="11"/>
+      <c r="D59" s="12"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="14">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="11"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="14">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="11"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="14">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="11"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="14">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C63" s="16"/>
-      <c r="D63" s="12"/>
+        <v>74</v>
+      </c>
+      <c r="C63" s="15"/>
+      <c r="D63" s="11"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="14">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C65" s="15"/>
+        <v>34</v>
+      </c>
+      <c r="C65" s="16"/>
       <c r="D65" s="12"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="14">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="14">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="C67" s="15"/>
       <c r="D67" s="12"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C68" s="15"/>
       <c r="D68" s="11"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="14">
-        <v>206</v>
+        <v>168</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="C69" s="15"/>
-      <c r="D69" s="11"/>
+      <c r="D69" s="12"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="14">
-        <v>215</v>
+        <v>169</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C70" s="16"/>
-      <c r="D70" s="12"/>
+        <v>86</v>
+      </c>
+      <c r="C70" s="15"/>
+      <c r="D70" s="11"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="14">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C71" s="23"/>
-      <c r="D71" s="12"/>
+      <c r="D71" s="11"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="14">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C72" s="16"/>
-      <c r="D72" s="13"/>
+      <c r="D72" s="12"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="14">
-        <v>300</v>
+        <v>234</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C73" s="22"/>
-      <c r="D73" s="13"/>
+      <c r="D73" s="12"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="14">
-        <v>322</v>
+        <v>238</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C74" s="16"/>
       <c r="D74" s="13"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="14">
-        <v>373</v>
+        <v>300</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C75" s="16"/>
       <c r="D75" s="13"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="14">
-        <v>394</v>
+        <v>322</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C76" s="16"/>
-      <c r="D76" s="12"/>
+      <c r="D76" s="13"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="14">
-        <v>647</v>
+        <v>373</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C77" s="16"/>
-      <c r="D77" s="12"/>
+      <c r="D77" s="13"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="14">
-        <v>1550</v>
+        <v>394</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C78" s="15"/>
-      <c r="D78" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="C78" s="16"/>
+      <c r="D78" s="12"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="14">
-        <v>1551</v>
+        <v>647</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="C79" s="16"/>
-      <c r="D79" s="11"/>
+      <c r="D79" s="12"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="14">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C80" s="16"/>
-      <c r="D80" s="13"/>
+        <v>63</v>
+      </c>
+      <c r="C80" s="15"/>
+      <c r="D80" s="11"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="14">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C81" s="17"/>
-      <c r="D81" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="C81" s="16"/>
+      <c r="D81" s="11"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="14">
-        <v>1556</v>
+        <v>1552</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C82" s="15"/>
-      <c r="D82" s="11"/>
+        <v>65</v>
+      </c>
+      <c r="C82" s="16"/>
+      <c r="D82" s="13"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="14">
-        <v>1557</v>
+        <v>1553</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C83" s="16"/>
+        <v>66</v>
+      </c>
+      <c r="C83" s="17"/>
       <c r="D83" s="12"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="14">
+        <v>1556</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C84" s="15"/>
+      <c r="D84" s="11"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="14">
+        <v>1557</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C85" s="16"/>
+      <c r="D85" s="12"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="14">
         <v>1558</v>
       </c>
-      <c r="B84" s="14" t="s">
+      <c r="B86" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="16"/>
-      <c r="D84" s="13"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="13"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D84">
-    <sortCondition ref="A64"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D86">
+    <sortCondition ref="A70"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Weekly Contest 204 - Problem 1566
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A83E1EB-F1C6-43F8-9ACC-014570BBAF95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA253E0-7FC9-411C-83DF-5B0A11421593}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>Group Anagrams</t>
+  </si>
+  <si>
+    <t>Detect Pattern of Length M Repeated K or More Times</t>
   </si>
 </sst>
 </file>
@@ -885,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1779,9 +1782,22 @@
       <c r="C86" s="16"/>
       <c r="D86" s="13"/>
     </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="14">
+        <v>1566</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C87" s="15"/>
+      <c r="D87" s="12"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C88"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D86">
-    <sortCondition ref="A70"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D88">
+    <sortCondition ref="A64"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Problem 42, 72 & 1143
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA253E0-7FC9-411C-83DF-5B0A11421593}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838226D3-4976-4F67-BB37-5A69C41C3DB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -301,6 +301,15 @@
   </si>
   <si>
     <t>Detect Pattern of Length M Repeated K or More Times</t>
+  </si>
+  <si>
+    <t>Edit Distance</t>
+  </si>
+  <si>
+    <t>Trapping Rain Water</t>
+  </si>
+  <si>
+    <t>Longest Common Subsequence</t>
   </si>
 </sst>
 </file>
@@ -502,7 +511,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -567,10 +576,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -888,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+      <selection activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1274,529 +1287,556 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="14">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="13"/>
+        <v>93</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="12"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="14">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C37" s="16"/>
-      <c r="D37" s="11"/>
+      <c r="D37" s="13"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="14">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C38" s="16"/>
       <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="14">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" s="16"/>
       <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="14">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="17"/>
-      <c r="D41" s="13"/>
+        <v>90</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="11"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="14">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="C42" s="17"/>
+      <c r="D42" s="13"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C43" s="15"/>
       <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="14">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C44" s="15"/>
       <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="14">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="14">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C46" s="15"/>
       <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="14">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C47" s="15"/>
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="14">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C48" s="15"/>
       <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="14">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="12"/>
+        <v>92</v>
+      </c>
+      <c r="C49" s="23"/>
+      <c r="D49" s="13"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="14">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C50" s="15"/>
-      <c r="D50" s="12"/>
+      <c r="D50" s="11"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="D51" s="11"/>
+      <c r="D51" s="12"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="14">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C52" s="15"/>
-      <c r="D52" s="11"/>
+      <c r="D52" s="12"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="14">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="D53" s="12"/>
+      <c r="D53" s="11"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="11"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="14">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C55" s="15"/>
       <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="14">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C56" s="15"/>
       <c r="D56" s="11"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="14">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C57" s="15"/>
-      <c r="D57" s="11"/>
+      <c r="D57" s="12"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="14">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C58" s="15"/>
-      <c r="D58" s="12"/>
+      <c r="D58" s="11"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="14">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C59" s="15"/>
-      <c r="D59" s="12"/>
+      <c r="D59" s="11"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="14">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C60" s="15"/>
-      <c r="D60" s="11"/>
+      <c r="D60" s="12"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="14">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C61" s="15"/>
-      <c r="D61" s="11"/>
+      <c r="D61" s="12"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="14">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="11"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="14">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="11"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="14">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C65" s="16"/>
-      <c r="D65" s="12"/>
+        <v>74</v>
+      </c>
+      <c r="C65" s="15"/>
+      <c r="D65" s="11"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="14">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="14">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C67" s="15"/>
+        <v>34</v>
+      </c>
+      <c r="C67" s="16"/>
       <c r="D67" s="12"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C68" s="15"/>
       <c r="D68" s="11"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="14">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="C69" s="15"/>
       <c r="D69" s="12"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="14">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C70" s="15"/>
       <c r="D70" s="11"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="14">
-        <v>206</v>
+        <v>168</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C71" s="23"/>
-      <c r="D71" s="11"/>
+        <v>85</v>
+      </c>
+      <c r="C71" s="22"/>
+      <c r="D71" s="12"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="14">
-        <v>215</v>
+        <v>169</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C72" s="16"/>
-      <c r="D72" s="12"/>
+        <v>86</v>
+      </c>
+      <c r="C72" s="15"/>
+      <c r="D72" s="11"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="14">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C73" s="22"/>
-      <c r="D73" s="12"/>
+      <c r="D73" s="11"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="14">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C74" s="16"/>
-      <c r="D74" s="13"/>
+      <c r="D74" s="12"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="14">
-        <v>300</v>
+        <v>234</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C75" s="16"/>
-      <c r="D75" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="C75" s="25"/>
+      <c r="D75" s="12"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="14">
-        <v>322</v>
+        <v>238</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C76" s="16"/>
       <c r="D76" s="13"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="14">
-        <v>373</v>
+        <v>300</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C77" s="16"/>
       <c r="D77" s="13"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="14">
-        <v>394</v>
+        <v>322</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C78" s="16"/>
-      <c r="D78" s="12"/>
+      <c r="D78" s="13"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="14">
-        <v>647</v>
+        <v>373</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C79" s="16"/>
-      <c r="D79" s="12"/>
+      <c r="D79" s="13"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="14">
-        <v>1550</v>
+        <v>394</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C80" s="15"/>
-      <c r="D80" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="C80" s="16"/>
+      <c r="D80" s="12"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="14">
-        <v>1551</v>
+        <v>647</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="C81" s="16"/>
-      <c r="D81" s="11"/>
+      <c r="D81" s="12"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="14">
-        <v>1552</v>
+        <v>1143</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C82" s="16"/>
-      <c r="D82" s="13"/>
+      <c r="D82" s="11"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="14">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C83" s="17"/>
-      <c r="D83" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="C83" s="15"/>
+      <c r="D83" s="11"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="14">
-        <v>1556</v>
+        <v>1551</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C84" s="15"/>
+        <v>64</v>
+      </c>
+      <c r="C84" s="16"/>
       <c r="D84" s="11"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="14">
-        <v>1557</v>
+        <v>1552</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C85" s="16"/>
-      <c r="D85" s="12"/>
+      <c r="D85" s="13"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="14">
-        <v>1558</v>
+        <v>1553</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C86" s="16"/>
-      <c r="D86" s="13"/>
+        <v>66</v>
+      </c>
+      <c r="C86" s="17"/>
+      <c r="D86" s="12"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="14">
+        <v>1556</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C87" s="15"/>
+      <c r="D87" s="11"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="14">
+        <v>1557</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C88" s="24"/>
+      <c r="D88" s="12"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="14">
+        <v>1558</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C89" s="16"/>
+      <c r="D89" s="13"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="14">
         <v>1566</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B90" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C87" s="15"/>
-      <c r="D87" s="12"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C88"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="12"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D88">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D90">
     <sortCondition ref="A64"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Problem 208, 226 & 1151
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838226D3-4976-4F67-BB37-5A69C41C3DB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4267F900-6968-4D41-9F8C-D5EA1AFB6B74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -310,6 +310,15 @@
   </si>
   <si>
     <t>Longest Common Subsequence</t>
+  </si>
+  <si>
+    <t>Minimum Swaps to Group All 1's Together</t>
+  </si>
+  <si>
+    <t>Implement Trie(Prefix tree)</t>
+  </si>
+  <si>
+    <t>Invert Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -901,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="J70" sqref="J70"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1667,177 +1676,207 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="14">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="C74" s="16"/>
       <c r="D74" s="12"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="14">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C75" s="25"/>
+        <v>37</v>
+      </c>
+      <c r="C75" s="16"/>
       <c r="D75" s="12"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="14">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C76" s="16"/>
-      <c r="D76" s="13"/>
+        <v>97</v>
+      </c>
+      <c r="C76" s="15"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="14">
-        <v>300</v>
+        <v>234</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C77" s="16"/>
-      <c r="D77" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="C77" s="25"/>
+      <c r="D77" s="12"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="14">
-        <v>322</v>
+        <v>238</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C78" s="16"/>
       <c r="D78" s="13"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="14">
-        <v>373</v>
+        <v>300</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C79" s="16"/>
       <c r="D79" s="13"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="14">
-        <v>394</v>
+        <v>322</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C80" s="16"/>
-      <c r="D80" s="12"/>
+      <c r="D80" s="13"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="14">
-        <v>647</v>
+        <v>373</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C81" s="16"/>
-      <c r="D81" s="12"/>
+      <c r="D81" s="13"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="14">
-        <v>1143</v>
+        <v>394</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="C82" s="16"/>
-      <c r="D82" s="11"/>
+      <c r="D82" s="12"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="14">
-        <v>1550</v>
+        <v>647</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C83" s="15"/>
-      <c r="D83" s="11"/>
+        <v>44</v>
+      </c>
+      <c r="C83" s="16"/>
+      <c r="D83" s="12"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="14">
-        <v>1551</v>
+        <v>1143</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="C84" s="16"/>
       <c r="D84" s="11"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="14">
-        <v>1552</v>
+        <v>1151</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="C85" s="16"/>
-      <c r="D85" s="13"/>
+      <c r="D85" s="12"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="14">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C86" s="17"/>
-      <c r="D86" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="C86" s="15"/>
+      <c r="D86" s="11"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="14">
-        <v>1556</v>
+        <v>1551</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C87" s="15"/>
+        <v>64</v>
+      </c>
+      <c r="C87" s="16"/>
       <c r="D87" s="11"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="14">
-        <v>1557</v>
+        <v>1552</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C88" s="24"/>
-      <c r="D88" s="12"/>
+      <c r="D88" s="13"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="14">
-        <v>1558</v>
+        <v>1553</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C89" s="16"/>
-      <c r="D89" s="13"/>
+        <v>66</v>
+      </c>
+      <c r="C89" s="17"/>
+      <c r="D89" s="12"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="14">
+        <v>1556</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C90" s="15"/>
+      <c r="D90" s="11"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="14">
+        <v>1557</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C91" s="16"/>
+      <c r="D91" s="12"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="14">
+        <v>1558</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C92" s="16"/>
+      <c r="D92" s="13"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="14">
         <v>1566</v>
       </c>
-      <c r="B90" s="14" t="s">
+      <c r="B93" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C90" s="15"/>
-      <c r="D90" s="12"/>
+      <c r="C93" s="15"/>
+      <c r="D93" s="12"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D90">
-    <sortCondition ref="A64"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D93">
+    <sortCondition ref="A70"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Problem 200, 253 & 518
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4267F900-6968-4D41-9F8C-D5EA1AFB6B74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EDB6DE-CF46-4B9C-AD6D-229FEB92BE03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -319,13 +319,22 @@
   </si>
   <si>
     <t>Invert Binary Tree</t>
+  </si>
+  <si>
+    <t>Number of Islands</t>
+  </si>
+  <si>
+    <t>Meeting Rooms II</t>
+  </si>
+  <si>
+    <t>Coin Change 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,18 +366,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Bahnschrift"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Bahnschrift"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="Bahnschrift"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -400,7 +413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -471,13 +484,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -486,8 +499,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -499,11 +514,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
@@ -520,26 +546,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -552,16 +566,28 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
@@ -573,26 +599,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -910,973 +930,1003 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="G83" sqref="G83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="47.77734375" style="14" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" style="18" customWidth="1"/>
-    <col min="4" max="4" width="24.21875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="59.5546875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" style="13" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:10" s="7" customFormat="1" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="14">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="15"/>
-      <c r="D2" s="11"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="3" t="s">
+      <c r="D2" s="15"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="14">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="16"/>
-      <c r="D3" s="12"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="4" t="s">
+      <c r="D3" s="16"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="16"/>
-      <c r="D4" s="13"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="6" t="s">
+      <c r="D4" s="17"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="14">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="17"/>
-      <c r="D5" s="13"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="8"/>
+      <c r="D5" s="17"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="12"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="14">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="16"/>
-      <c r="D7" s="13"/>
+      <c r="D7" s="17"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="14">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="15"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="14">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="16"/>
-      <c r="D9" s="12"/>
+      <c r="D9" s="16"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="14">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="11"/>
+      <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
+      <c r="A11" s="13">
         <v>11</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="16"/>
-      <c r="D11" s="12"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
+      <c r="A12" s="13">
         <v>12</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="16"/>
-      <c r="D12" s="12"/>
+      <c r="D12" s="16"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
+      <c r="A13" s="13">
         <v>13</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="15"/>
-      <c r="D13" s="12"/>
+      <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="14">
+      <c r="A14" s="13">
         <v>14</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="15"/>
-      <c r="D14" s="12"/>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="14">
+      <c r="A15" s="13">
         <v>15</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="16"/>
-      <c r="D15" s="12"/>
+      <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="14">
+      <c r="A16" s="13">
         <v>16</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="16"/>
-      <c r="D16" s="12"/>
+      <c r="D16" s="16"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="14">
+      <c r="A17" s="13">
         <v>17</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C17" s="16"/>
-      <c r="D17" s="11"/>
+      <c r="D17" s="15"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="14">
+      <c r="A18" s="13">
         <v>18</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>56</v>
       </c>
       <c r="C18" s="16"/>
-      <c r="D18" s="12"/>
+      <c r="D18" s="16"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="14">
+      <c r="A19" s="13">
         <v>19</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>58</v>
       </c>
       <c r="C19" s="16"/>
-      <c r="D19" s="11"/>
+      <c r="D19" s="15"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="14">
+      <c r="A20" s="13">
         <v>20</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="15"/>
-      <c r="D20" s="11"/>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="14">
+      <c r="A21" s="13">
         <v>21</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="15"/>
-      <c r="D21" s="12"/>
+      <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="14">
+      <c r="A22" s="13">
         <v>22</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>62</v>
       </c>
       <c r="C22" s="16"/>
-      <c r="D22" s="12"/>
+      <c r="D22" s="16"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="14">
+      <c r="A23" s="13">
         <v>24</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>59</v>
       </c>
       <c r="C23" s="16"/>
-      <c r="D23" s="12"/>
+      <c r="D23" s="16"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="14">
+      <c r="A24" s="13">
         <v>26</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="15"/>
-      <c r="D24" s="12"/>
+      <c r="D24" s="16"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
+      <c r="A25" s="13">
         <v>27</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="15"/>
-      <c r="D25" s="12"/>
+      <c r="D25" s="16"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="14">
+      <c r="A26" s="13">
         <v>28</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="15"/>
-      <c r="D26" s="11"/>
+      <c r="D26" s="15"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="14">
+      <c r="A27" s="13">
         <v>29</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>60</v>
       </c>
       <c r="C27" s="16"/>
-      <c r="D27" s="13"/>
+      <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="14">
+      <c r="A28" s="13">
         <v>31</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>61</v>
       </c>
       <c r="C28" s="16"/>
-      <c r="D28" s="13"/>
+      <c r="D28" s="17"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="14">
+      <c r="A29" s="13">
         <v>33</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>76</v>
       </c>
       <c r="C29" s="16"/>
-      <c r="D29" s="12"/>
+      <c r="D29" s="16"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="14">
+      <c r="A30" s="13">
         <v>34</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C30" s="16"/>
-      <c r="D30" s="12"/>
+      <c r="D30" s="16"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="14">
+      <c r="A31" s="13">
         <v>35</v>
       </c>
       <c r="B31" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C31" s="15"/>
-      <c r="D31" s="11"/>
+      <c r="D31" s="15"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="14">
+      <c r="A32" s="13">
         <v>36</v>
       </c>
       <c r="B32" s="14" t="s">
         <v>77</v>
       </c>
       <c r="C32" s="16"/>
-      <c r="D32" s="12"/>
+      <c r="D32" s="16"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="14">
+      <c r="A33" s="13">
         <v>38</v>
       </c>
       <c r="B33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="17"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="14">
+      <c r="A34" s="13">
         <v>39</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>78</v>
       </c>
       <c r="C34" s="16"/>
-      <c r="D34" s="13"/>
+      <c r="D34" s="17"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="14">
+      <c r="A35" s="13">
         <v>40</v>
       </c>
       <c r="B35" s="14" t="s">
         <v>78</v>
       </c>
       <c r="C35" s="16"/>
-      <c r="D35" s="13"/>
+      <c r="D35" s="17"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="14">
+      <c r="A36" s="13">
         <v>42</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>93</v>
       </c>
       <c r="C36" s="17"/>
-      <c r="D36" s="12"/>
+      <c r="D36" s="16"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="14">
+      <c r="A37" s="13">
         <v>43</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>79</v>
       </c>
       <c r="C37" s="16"/>
-      <c r="D37" s="13"/>
+      <c r="D37" s="17"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="14">
+      <c r="A38" s="13">
         <v>46</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>87</v>
       </c>
       <c r="C38" s="16"/>
-      <c r="D38" s="11"/>
+      <c r="D38" s="15"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="14">
+      <c r="A39" s="13">
         <v>47</v>
       </c>
       <c r="B39" s="14" t="s">
         <v>88</v>
       </c>
       <c r="C39" s="16"/>
-      <c r="D39" s="11"/>
+      <c r="D39" s="15"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="14">
+      <c r="A40" s="13">
         <v>48</v>
       </c>
       <c r="B40" s="14" t="s">
         <v>89</v>
       </c>
       <c r="C40" s="16"/>
-      <c r="D40" s="11"/>
+      <c r="D40" s="15"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="14">
+      <c r="A41" s="13">
         <v>49</v>
       </c>
       <c r="B41" s="14" t="s">
         <v>90</v>
       </c>
       <c r="C41" s="16"/>
-      <c r="D41" s="11"/>
+      <c r="D41" s="15"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="14">
+      <c r="A42" s="13">
         <v>51</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>52</v>
       </c>
       <c r="C42" s="17"/>
-      <c r="D42" s="13"/>
+      <c r="D42" s="17"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="14">
+      <c r="A43" s="13">
         <v>53</v>
       </c>
       <c r="B43" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C43" s="15"/>
-      <c r="D43" s="11"/>
+      <c r="D43" s="15"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="14">
+      <c r="A44" s="13">
         <v>58</v>
       </c>
       <c r="B44" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C44" s="15"/>
-      <c r="D44" s="11"/>
+      <c r="D44" s="15"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="14">
+      <c r="A45" s="13">
         <v>66</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C45" s="15"/>
-      <c r="D45" s="11"/>
+      <c r="D45" s="15"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="14">
+      <c r="A46" s="13">
         <v>67</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C46" s="15"/>
-      <c r="D46" s="11"/>
+      <c r="D46" s="15"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="14">
+      <c r="A47" s="13">
         <v>69</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="D47" s="11"/>
+      <c r="D47" s="15"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="14">
+      <c r="A48" s="13">
         <v>70</v>
       </c>
       <c r="B48" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C48" s="15"/>
-      <c r="D48" s="11"/>
+      <c r="D48" s="15"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="14">
+      <c r="A49" s="13">
         <v>72</v>
       </c>
       <c r="B49" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C49" s="23"/>
-      <c r="D49" s="13"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="17"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="14">
+      <c r="A50" s="13">
         <v>83</v>
       </c>
       <c r="B50" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C50" s="15"/>
-      <c r="D50" s="11"/>
+      <c r="D50" s="15"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="14">
+      <c r="A51" s="13">
         <v>88</v>
       </c>
       <c r="B51" s="14" t="s">
         <v>32</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="D51" s="12"/>
+      <c r="D51" s="16"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="14">
+      <c r="A52" s="13">
         <v>100</v>
       </c>
       <c r="B52" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C52" s="15"/>
-      <c r="D52" s="12"/>
+      <c r="D52" s="16"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="14">
+      <c r="A53" s="13">
         <v>101</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="D53" s="11"/>
+      <c r="D53" s="15"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="14">
+      <c r="A54" s="13">
         <v>104</v>
       </c>
       <c r="B54" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C54" s="15"/>
-      <c r="D54" s="11"/>
+      <c r="D54" s="15"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="14">
+      <c r="A55" s="13">
         <v>107</v>
       </c>
       <c r="B55" s="14" t="s">
         <v>47</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="D55" s="12"/>
+      <c r="D55" s="16"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="14">
+      <c r="A56" s="13">
         <v>108</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C56" s="15"/>
-      <c r="D56" s="11"/>
+      <c r="D56" s="15"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="14">
+      <c r="A57" s="13">
         <v>110</v>
       </c>
       <c r="B57" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C57" s="15"/>
-      <c r="D57" s="12"/>
+      <c r="D57" s="16"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="14">
+      <c r="A58" s="13">
         <v>111</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>67</v>
       </c>
       <c r="C58" s="15"/>
-      <c r="D58" s="11"/>
+      <c r="D58" s="15"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="14">
+      <c r="A59" s="13">
         <v>112</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C59" s="15"/>
-      <c r="D59" s="11"/>
+      <c r="D59" s="15"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="14">
+      <c r="A60" s="13">
         <v>118</v>
       </c>
       <c r="B60" s="14" t="s">
         <v>69</v>
       </c>
       <c r="C60" s="15"/>
-      <c r="D60" s="12"/>
+      <c r="D60" s="16"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="14">
+      <c r="A61" s="13">
         <v>119</v>
       </c>
       <c r="B61" s="14" t="s">
         <v>70</v>
       </c>
       <c r="C61" s="15"/>
-      <c r="D61" s="12"/>
+      <c r="D61" s="16"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="14">
+      <c r="A62" s="13">
         <v>121</v>
       </c>
       <c r="B62" s="14" t="s">
         <v>71</v>
       </c>
       <c r="C62" s="15"/>
-      <c r="D62" s="11"/>
+      <c r="D62" s="15"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="14">
+      <c r="A63" s="13">
         <v>122</v>
       </c>
       <c r="B63" s="14" t="s">
         <v>72</v>
       </c>
       <c r="C63" s="15"/>
-      <c r="D63" s="11"/>
+      <c r="D63" s="15"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="14">
+      <c r="A64" s="13">
         <v>125</v>
       </c>
       <c r="B64" s="14" t="s">
         <v>73</v>
       </c>
       <c r="C64" s="15"/>
-      <c r="D64" s="11"/>
+      <c r="D64" s="15"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="14">
+      <c r="A65" s="13">
         <v>136</v>
       </c>
       <c r="B65" s="14" t="s">
         <v>74</v>
       </c>
       <c r="C65" s="15"/>
-      <c r="D65" s="11"/>
+      <c r="D65" s="15"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="14">
+      <c r="A66" s="13">
         <v>141</v>
       </c>
       <c r="B66" s="14" t="s">
         <v>75</v>
       </c>
       <c r="C66" s="15"/>
-      <c r="D66" s="11"/>
+      <c r="D66" s="15"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="14">
+      <c r="A67" s="13">
         <v>152</v>
       </c>
       <c r="B67" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C67" s="16"/>
-      <c r="D67" s="12"/>
+      <c r="D67" s="16"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="14">
+      <c r="A68" s="13">
         <v>155</v>
       </c>
       <c r="B68" s="14" t="s">
         <v>83</v>
       </c>
       <c r="C68" s="15"/>
-      <c r="D68" s="11"/>
+      <c r="D68" s="15"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="14">
+      <c r="A69" s="13">
         <v>160</v>
       </c>
       <c r="B69" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C69" s="15"/>
-      <c r="D69" s="12"/>
+      <c r="D69" s="16"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="14">
+      <c r="A70" s="13">
         <v>167</v>
       </c>
       <c r="B70" s="14" t="s">
         <v>84</v>
       </c>
       <c r="C70" s="15"/>
-      <c r="D70" s="11"/>
+      <c r="D70" s="15"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="14">
+      <c r="A71" s="13">
         <v>168</v>
       </c>
       <c r="B71" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C71" s="22"/>
-      <c r="D71" s="12"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="16"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="14">
+      <c r="A72" s="13">
         <v>169</v>
       </c>
       <c r="B72" s="14" t="s">
         <v>86</v>
       </c>
       <c r="C72" s="15"/>
-      <c r="D72" s="11"/>
+      <c r="D72" s="15"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="14">
+      <c r="A73" s="13">
+        <v>200</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C73" s="21"/>
+      <c r="D73" s="15"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="13">
         <v>206</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B74" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C73" s="22"/>
-      <c r="D73" s="11"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="14">
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="13">
         <v>208</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B75" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C74" s="16"/>
-      <c r="D74" s="12"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="14">
+      <c r="C75" s="16"/>
+      <c r="D75" s="16"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="13">
         <v>215</v>
       </c>
-      <c r="B75" s="14" t="s">
+      <c r="B76" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C75" s="16"/>
-      <c r="D75" s="12"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="14">
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="13">
         <v>226</v>
       </c>
-      <c r="B76" s="14" t="s">
+      <c r="B77" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C76" s="15"/>
-      <c r="D76" s="11"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="14">
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="13">
         <v>234</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B78" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C77" s="25"/>
-      <c r="D77" s="12"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="14">
+      <c r="C78" s="22"/>
+      <c r="D78" s="16"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="13">
         <v>238</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B79" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C78" s="16"/>
-      <c r="D78" s="13"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="14">
+      <c r="C79" s="16"/>
+      <c r="D79" s="17"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="13">
+        <v>253</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="13">
         <v>300</v>
       </c>
-      <c r="B79" s="14" t="s">
+      <c r="B81" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C79" s="16"/>
-      <c r="D79" s="13"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="14">
+      <c r="C81" s="16"/>
+      <c r="D81" s="17"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="13">
         <v>322</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B82" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C80" s="16"/>
-      <c r="D80" s="13"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="14">
+      <c r="C82" s="16"/>
+      <c r="D82" s="17"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="13">
         <v>373</v>
       </c>
-      <c r="B81" s="14" t="s">
+      <c r="B83" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C81" s="16"/>
-      <c r="D81" s="13"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="14">
+      <c r="C83" s="16"/>
+      <c r="D83" s="17"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="13">
         <v>394</v>
       </c>
-      <c r="B82" s="14" t="s">
+      <c r="B84" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C82" s="16"/>
-      <c r="D82" s="12"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="14">
+      <c r="C84" s="16"/>
+      <c r="D84" s="16"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="13">
+        <v>518</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C85" s="16"/>
+      <c r="D85" s="16"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="13">
         <v>647</v>
       </c>
-      <c r="B83" s="14" t="s">
+      <c r="B86" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C83" s="16"/>
-      <c r="D83" s="12"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="14">
+      <c r="C86" s="16"/>
+      <c r="D86" s="16"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="13">
         <v>1143</v>
       </c>
-      <c r="B84" s="14" t="s">
+      <c r="B87" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C84" s="16"/>
-      <c r="D84" s="11"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="14">
+      <c r="C87" s="16"/>
+      <c r="D87" s="15"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="13">
         <v>1151</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B88" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C85" s="16"/>
-      <c r="D85" s="12"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="14">
+      <c r="C88" s="23"/>
+      <c r="D88" s="16"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="13">
         <v>1550</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B89" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C86" s="15"/>
-      <c r="D86" s="11"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="14">
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="13">
         <v>1551</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B90" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C87" s="16"/>
-      <c r="D87" s="11"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="14">
+      <c r="C90" s="16"/>
+      <c r="D90" s="15"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="13">
         <v>1552</v>
       </c>
-      <c r="B88" s="14" t="s">
+      <c r="B91" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C88" s="24"/>
-      <c r="D88" s="13"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="14">
+      <c r="C91" s="16"/>
+      <c r="D91" s="17"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="13">
         <v>1553</v>
       </c>
-      <c r="B89" s="14" t="s">
+      <c r="B92" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C89" s="17"/>
-      <c r="D89" s="12"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="14">
+      <c r="C92" s="17"/>
+      <c r="D92" s="16"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="13">
         <v>1556</v>
       </c>
-      <c r="B90" s="14" t="s">
+      <c r="B93" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C90" s="15"/>
-      <c r="D90" s="11"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="14">
+      <c r="C93" s="15"/>
+      <c r="D93" s="15"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="13">
         <v>1557</v>
       </c>
-      <c r="B91" s="14" t="s">
+      <c r="B94" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C91" s="16"/>
-      <c r="D91" s="12"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="14">
+      <c r="C94" s="16"/>
+      <c r="D94" s="16"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="13">
         <v>1558</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B95" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C92" s="16"/>
-      <c r="D92" s="13"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="14">
+      <c r="C95" s="16"/>
+      <c r="D95" s="17"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="13">
         <v>1566</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="B96" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C93" s="15"/>
-      <c r="D93" s="12"/>
+      <c r="C96" s="15"/>
+      <c r="D96" s="16"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D93">
-    <sortCondition ref="A70"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D96">
+    <sortCondition ref="A82"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Problem 78, 286 & 295
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EDB6DE-CF46-4B9C-AD6D-229FEB92BE03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30779A6D-B387-4B2E-856B-319C612E3BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -328,6 +328,15 @@
   </si>
   <si>
     <t>Coin Change 2</t>
+  </si>
+  <si>
+    <t>Subsets</t>
+  </si>
+  <si>
+    <t>Walls and Gates</t>
+  </si>
+  <si>
+    <t>Find Median from Data Stream</t>
   </si>
 </sst>
 </file>
@@ -546,7 +555,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -604,9 +613,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
@@ -930,15 +936,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J96"/>
+  <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A82" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" style="14" customWidth="1"/>
     <col min="2" max="2" width="59.5546875" style="14" customWidth="1"/>
     <col min="3" max="3" width="23.77734375" style="13" customWidth="1"/>
     <col min="4" max="4" width="24.21875" style="13" customWidth="1"/>
@@ -961,7 +967,7 @@
       <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -975,7 +981,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="14">
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -989,7 +995,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13">
+      <c r="A4" s="14">
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
@@ -1003,7 +1009,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="14">
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -1015,7 +1021,7 @@
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="14">
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -1025,7 +1031,7 @@
       <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="14">
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -1035,7 +1041,7 @@
       <c r="D7" s="17"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="14">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
@@ -1045,7 +1051,7 @@
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="14">
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -1055,7 +1061,7 @@
       <c r="D9" s="16"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="14">
         <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
@@ -1065,7 +1071,7 @@
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11" s="14">
         <v>11</v>
       </c>
       <c r="B11" s="14" t="s">
@@ -1075,7 +1081,7 @@
       <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12" s="14">
         <v>12</v>
       </c>
       <c r="B12" s="14" t="s">
@@ -1085,7 +1091,7 @@
       <c r="D12" s="16"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="14">
         <v>13</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -1095,7 +1101,7 @@
       <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="13">
+      <c r="A14" s="14">
         <v>14</v>
       </c>
       <c r="B14" s="14" t="s">
@@ -1105,7 +1111,7 @@
       <c r="D14" s="16"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="13">
+      <c r="A15" s="14">
         <v>15</v>
       </c>
       <c r="B15" s="14" t="s">
@@ -1115,7 +1121,7 @@
       <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="13">
+      <c r="A16" s="14">
         <v>16</v>
       </c>
       <c r="B16" s="14" t="s">
@@ -1125,7 +1131,7 @@
       <c r="D16" s="16"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="13">
+      <c r="A17" s="14">
         <v>17</v>
       </c>
       <c r="B17" s="14" t="s">
@@ -1135,7 +1141,7 @@
       <c r="D17" s="15"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="13">
+      <c r="A18" s="14">
         <v>18</v>
       </c>
       <c r="B18" s="14" t="s">
@@ -1145,7 +1151,7 @@
       <c r="D18" s="16"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="13">
+      <c r="A19" s="14">
         <v>19</v>
       </c>
       <c r="B19" s="14" t="s">
@@ -1155,7 +1161,7 @@
       <c r="D19" s="15"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="13">
+      <c r="A20" s="14">
         <v>20</v>
       </c>
       <c r="B20" s="14" t="s">
@@ -1165,7 +1171,7 @@
       <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="13">
+      <c r="A21" s="14">
         <v>21</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -1175,7 +1181,7 @@
       <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="13">
+      <c r="A22" s="14">
         <v>22</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -1185,7 +1191,7 @@
       <c r="D22" s="16"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="13">
+      <c r="A23" s="14">
         <v>24</v>
       </c>
       <c r="B23" s="14" t="s">
@@ -1195,7 +1201,7 @@
       <c r="D23" s="16"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="13">
+      <c r="A24" s="14">
         <v>26</v>
       </c>
       <c r="B24" s="14" t="s">
@@ -1205,7 +1211,7 @@
       <c r="D24" s="16"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="13">
+      <c r="A25" s="14">
         <v>27</v>
       </c>
       <c r="B25" s="14" t="s">
@@ -1215,7 +1221,7 @@
       <c r="D25" s="16"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="13">
+      <c r="A26" s="14">
         <v>28</v>
       </c>
       <c r="B26" s="14" t="s">
@@ -1225,7 +1231,7 @@
       <c r="D26" s="15"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="13">
+      <c r="A27" s="14">
         <v>29</v>
       </c>
       <c r="B27" s="14" t="s">
@@ -1235,7 +1241,7 @@
       <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="13">
+      <c r="A28" s="14">
         <v>31</v>
       </c>
       <c r="B28" s="14" t="s">
@@ -1245,7 +1251,7 @@
       <c r="D28" s="17"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="13">
+      <c r="A29" s="14">
         <v>33</v>
       </c>
       <c r="B29" s="14" t="s">
@@ -1255,7 +1261,7 @@
       <c r="D29" s="16"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="13">
+      <c r="A30" s="14">
         <v>34</v>
       </c>
       <c r="B30" s="14" t="s">
@@ -1265,7 +1271,7 @@
       <c r="D30" s="16"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="13">
+      <c r="A31" s="14">
         <v>35</v>
       </c>
       <c r="B31" s="14" t="s">
@@ -1275,7 +1281,7 @@
       <c r="D31" s="15"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="13">
+      <c r="A32" s="14">
         <v>36</v>
       </c>
       <c r="B32" s="14" t="s">
@@ -1285,7 +1291,7 @@
       <c r="D32" s="16"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="13">
+      <c r="A33" s="14">
         <v>38</v>
       </c>
       <c r="B33" s="14" t="s">
@@ -1295,7 +1301,7 @@
       <c r="D33" s="17"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="13">
+      <c r="A34" s="14">
         <v>39</v>
       </c>
       <c r="B34" s="14" t="s">
@@ -1305,7 +1311,7 @@
       <c r="D34" s="17"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="13">
+      <c r="A35" s="14">
         <v>40</v>
       </c>
       <c r="B35" s="14" t="s">
@@ -1315,7 +1321,7 @@
       <c r="D35" s="17"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="13">
+      <c r="A36" s="14">
         <v>42</v>
       </c>
       <c r="B36" s="14" t="s">
@@ -1325,7 +1331,7 @@
       <c r="D36" s="16"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="13">
+      <c r="A37" s="14">
         <v>43</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -1335,7 +1341,7 @@
       <c r="D37" s="17"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="13">
+      <c r="A38" s="14">
         <v>46</v>
       </c>
       <c r="B38" s="14" t="s">
@@ -1345,7 +1351,7 @@
       <c r="D38" s="15"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="13">
+      <c r="A39" s="14">
         <v>47</v>
       </c>
       <c r="B39" s="14" t="s">
@@ -1355,7 +1361,7 @@
       <c r="D39" s="15"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="13">
+      <c r="A40" s="14">
         <v>48</v>
       </c>
       <c r="B40" s="14" t="s">
@@ -1365,7 +1371,7 @@
       <c r="D40" s="15"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="13">
+      <c r="A41" s="14">
         <v>49</v>
       </c>
       <c r="B41" s="14" t="s">
@@ -1375,7 +1381,7 @@
       <c r="D41" s="15"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="13">
+      <c r="A42" s="14">
         <v>51</v>
       </c>
       <c r="B42" s="14" t="s">
@@ -1385,7 +1391,7 @@
       <c r="D42" s="17"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="13">
+      <c r="A43" s="14">
         <v>53</v>
       </c>
       <c r="B43" s="14" t="s">
@@ -1395,7 +1401,7 @@
       <c r="D43" s="15"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="13">
+      <c r="A44" s="14">
         <v>58</v>
       </c>
       <c r="B44" s="14" t="s">
@@ -1405,7 +1411,7 @@
       <c r="D44" s="15"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="13">
+      <c r="A45" s="14">
         <v>66</v>
       </c>
       <c r="B45" s="14" t="s">
@@ -1415,7 +1421,7 @@
       <c r="D45" s="15"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="13">
+      <c r="A46" s="14">
         <v>67</v>
       </c>
       <c r="B46" s="14" t="s">
@@ -1425,7 +1431,7 @@
       <c r="D46" s="15"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="13">
+      <c r="A47" s="14">
         <v>69</v>
       </c>
       <c r="B47" s="14" t="s">
@@ -1435,7 +1441,7 @@
       <c r="D47" s="15"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="13">
+      <c r="A48" s="14">
         <v>70</v>
       </c>
       <c r="B48" s="14" t="s">
@@ -1445,7 +1451,7 @@
       <c r="D48" s="15"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="13">
+      <c r="A49" s="14">
         <v>72</v>
       </c>
       <c r="B49" s="14" t="s">
@@ -1455,477 +1461,507 @@
       <c r="D49" s="17"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="13">
+      <c r="A50" s="14">
+        <v>78</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="14">
         <v>83</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B51" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="13">
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="14">
         <v>88</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B52" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="16"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="13">
-        <v>100</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>33</v>
       </c>
       <c r="C52" s="15"/>
       <c r="D52" s="16"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="13">
+      <c r="A53" s="14">
+        <v>100</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="15"/>
+      <c r="D53" s="16"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="14">
         <v>101</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B54" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="13">
-        <v>104</v>
-      </c>
-      <c r="B54" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="13">
+      <c r="A55" s="14">
+        <v>104</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="14">
         <v>107</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B56" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C55" s="15"/>
-      <c r="D55" s="16"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="13">
+      <c r="C56" s="15"/>
+      <c r="D56" s="16"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="14">
         <v>108</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B57" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="13">
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="14">
         <v>110</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B58" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="16"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="13">
+      <c r="C58" s="15"/>
+      <c r="D58" s="16"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="14">
         <v>111</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B59" s="14" t="s">
         <v>67</v>
-      </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="13">
-        <v>112</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>68</v>
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="15"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="13">
+      <c r="A60" s="14">
+        <v>112</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="14">
         <v>118</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B61" s="14" t="s">
         <v>69</v>
-      </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="16"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="13">
-        <v>119</v>
-      </c>
-      <c r="B61" s="14" t="s">
-        <v>70</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="16"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="13">
+      <c r="A62" s="14">
+        <v>119</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="15"/>
+      <c r="D62" s="16"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="14">
         <v>121</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B63" s="14" t="s">
         <v>71</v>
-      </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="13">
-        <v>122</v>
-      </c>
-      <c r="B63" s="14" t="s">
-        <v>72</v>
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="13">
-        <v>125</v>
+      <c r="A64" s="14">
+        <v>122</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="15"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="13">
-        <v>136</v>
+      <c r="A65" s="14">
+        <v>125</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="13">
-        <v>141</v>
+      <c r="A66" s="14">
+        <v>136</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="13">
+      <c r="A67" s="14">
+        <v>141</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="14">
         <v>152</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B68" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="13">
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="14">
         <v>155</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B69" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="13">
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="14">
         <v>160</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B70" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C69" s="15"/>
-      <c r="D69" s="16"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="13">
+      <c r="C70" s="15"/>
+      <c r="D70" s="16"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="14">
         <v>167</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B71" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="13">
+      <c r="C71" s="20"/>
+      <c r="D71" s="15"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="14">
         <v>168</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B72" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C71" s="20"/>
-      <c r="D71" s="16"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="13">
+      <c r="C72" s="15"/>
+      <c r="D72" s="16"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="14">
         <v>169</v>
       </c>
-      <c r="B72" s="14" t="s">
+      <c r="B73" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="13">
+      <c r="C73" s="20"/>
+      <c r="D73" s="15"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="14">
         <v>200</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B74" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="C73" s="21"/>
-      <c r="D73" s="15"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="13">
+      <c r="C74" s="16"/>
+      <c r="D74" s="15"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="14">
         <v>206</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B75" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="13">
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="14">
         <v>208</v>
       </c>
-      <c r="B75" s="14" t="s">
+      <c r="B76" s="14" t="s">
         <v>96</v>
-      </c>
-      <c r="C75" s="16"/>
-      <c r="D75" s="16"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="13">
-        <v>215</v>
-      </c>
-      <c r="B76" s="14" t="s">
-        <v>37</v>
       </c>
       <c r="C76" s="16"/>
       <c r="D76" s="16"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="13">
+      <c r="A77" s="14">
+        <v>215</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C77" s="16"/>
+      <c r="D77" s="16"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="14">
         <v>226</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B78" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="13">
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="14">
         <v>234</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B79" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C78" s="22"/>
-      <c r="D78" s="16"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="13">
+      <c r="C79" s="21"/>
+      <c r="D79" s="16"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="14">
         <v>238</v>
       </c>
-      <c r="B79" s="14" t="s">
+      <c r="B80" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C79" s="16"/>
-      <c r="D79" s="17"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="13">
+      <c r="C80" s="16"/>
+      <c r="D80" s="17"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="14">
         <v>253</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B81" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C80" s="16"/>
-      <c r="D80" s="16"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="13">
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="14">
+        <v>286</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C82" s="16"/>
+      <c r="D82" s="16"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="14">
+        <v>295</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C83" s="17"/>
+      <c r="D83" s="17"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="14">
         <v>300</v>
       </c>
-      <c r="B81" s="14" t="s">
+      <c r="B84" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C81" s="16"/>
-      <c r="D81" s="17"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="13">
+      <c r="C84" s="16"/>
+      <c r="D84" s="17"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="14">
         <v>322</v>
       </c>
-      <c r="B82" s="14" t="s">
+      <c r="B85" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C82" s="16"/>
-      <c r="D82" s="17"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="13">
+      <c r="C85" s="16"/>
+      <c r="D85" s="17"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="14">
         <v>373</v>
       </c>
-      <c r="B83" s="14" t="s">
+      <c r="B86" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C83" s="16"/>
-      <c r="D83" s="17"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="13">
+      <c r="C86" s="16"/>
+      <c r="D86" s="17"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="14">
         <v>394</v>
       </c>
-      <c r="B84" s="14" t="s">
+      <c r="B87" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C84" s="16"/>
-      <c r="D84" s="16"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="13">
+      <c r="C87" s="16"/>
+      <c r="D87" s="16"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="14">
         <v>518</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B88" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C85" s="16"/>
-      <c r="D85" s="16"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="13">
+      <c r="C88" s="22"/>
+      <c r="D88" s="16"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="14">
         <v>647</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B89" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C86" s="16"/>
-      <c r="D86" s="16"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="13">
+      <c r="C89" s="16"/>
+      <c r="D89" s="16"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="14">
         <v>1143</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B90" s="14" t="s">
         <v>94</v>
-      </c>
-      <c r="C87" s="16"/>
-      <c r="D87" s="15"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="13">
-        <v>1151</v>
-      </c>
-      <c r="B88" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="C88" s="23"/>
-      <c r="D88" s="16"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="13">
-        <v>1550</v>
-      </c>
-      <c r="B89" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C89" s="15"/>
-      <c r="D89" s="15"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="13">
-        <v>1551</v>
-      </c>
-      <c r="B90" s="14" t="s">
-        <v>64</v>
       </c>
       <c r="C90" s="16"/>
       <c r="D90" s="15"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="13">
+      <c r="A91" s="14">
+        <v>1151</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C91" s="16"/>
+      <c r="D91" s="16"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="14">
+        <v>1550</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C92" s="15"/>
+      <c r="D92" s="15"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="14">
+        <v>1551</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C93" s="16"/>
+      <c r="D93" s="15"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="14">
         <v>1552</v>
       </c>
-      <c r="B91" s="14" t="s">
+      <c r="B94" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C91" s="16"/>
-      <c r="D91" s="17"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="13">
+      <c r="C94" s="16"/>
+      <c r="D94" s="17"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="14">
         <v>1553</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B95" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C92" s="17"/>
-      <c r="D92" s="16"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="13">
+      <c r="C95" s="17"/>
+      <c r="D95" s="16"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="14">
         <v>1556</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="B96" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C93" s="15"/>
-      <c r="D93" s="15"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="13">
+      <c r="C96" s="15"/>
+      <c r="D96" s="15"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="14">
         <v>1557</v>
       </c>
-      <c r="B94" s="14" t="s">
+      <c r="B97" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C94" s="16"/>
-      <c r="D94" s="16"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="13">
+      <c r="C97" s="16"/>
+      <c r="D97" s="16"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="14">
         <v>1558</v>
       </c>
-      <c r="B95" s="14" t="s">
+      <c r="B98" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C95" s="16"/>
-      <c r="D95" s="17"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="13">
+      <c r="C98" s="16"/>
+      <c r="D98" s="17"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="14">
         <v>1566</v>
       </c>
-      <c r="B96" s="14" t="s">
+      <c r="B99" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C96" s="15"/>
-      <c r="D96" s="16"/>
+      <c r="C99" s="15"/>
+      <c r="D99" s="16"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D96">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D99">
     <sortCondition ref="A82"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Biweekly Contest 34 (Problem 1572, 1573, 1574 & 1575)
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30779A6D-B387-4B2E-856B-319C612E3BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FBE174-F790-4264-8BD2-F69265208EA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -337,6 +337,18 @@
   </si>
   <si>
     <t>Find Median from Data Stream</t>
+  </si>
+  <si>
+    <t>Matrix Diagonal Sum</t>
+  </si>
+  <si>
+    <t>Number of Ways to Split a String</t>
+  </si>
+  <si>
+    <t>Shortest Subarray to be Removed to Make Array Sorted</t>
+  </si>
+  <si>
+    <t>Count All Possible Routes</t>
   </si>
 </sst>
 </file>
@@ -936,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J99"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A82" sqref="A1:A1048576"/>
+      <selection activeCell="K93" sqref="K93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1960,8 +1972,48 @@
       <c r="C99" s="15"/>
       <c r="D99" s="16"/>
     </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="14">
+        <v>1572</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C100" s="15"/>
+      <c r="D100" s="15"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="14">
+        <v>1573</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C101" s="16"/>
+      <c r="D101" s="16"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="14">
+        <v>1574</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C102" s="16"/>
+      <c r="D102" s="17"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="14">
+        <v>1575</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C103" s="17"/>
+      <c r="D103" s="17"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D99">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D103">
     <sortCondition ref="A82"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Weekly Contest 205 (Problem 1576, 1577 & 1578)
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FBE174-F790-4264-8BD2-F69265208EA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F65A66E-FCF4-4E18-B6E5-1F30572C0A70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
   <si>
     <t>Name</t>
   </si>
@@ -349,6 +349,15 @@
   </si>
   <si>
     <t>Count All Possible Routes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Replace All ?'s to Avoid Consecutive Repeating Characters</t>
+  </si>
+  <si>
+    <t>Number of Ways Where Square of Number Is Equal to Product of Two Numbers</t>
+  </si>
+  <si>
+    <t>Minimum Deletion Cost to Avoid Repeating Letters</t>
   </si>
 </sst>
 </file>
@@ -948,16 +957,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="K93" sqref="K93"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.5546875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="59.5546875" style="14" customWidth="1"/>
+    <col min="2" max="2" width="77.109375" style="14" customWidth="1"/>
     <col min="3" max="3" width="23.77734375" style="13" customWidth="1"/>
     <col min="4" max="4" width="24.21875" style="13" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
@@ -2012,6 +2021,39 @@
       <c r="C103" s="17"/>
       <c r="D103" s="17"/>
     </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="14">
+        <v>1576</v>
+      </c>
+      <c r="B104" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C104" s="15"/>
+      <c r="D104" s="16"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="14">
+        <v>1577</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C105" s="16"/>
+      <c r="D105" s="16"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="14">
+        <v>1578</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C106" s="16"/>
+      <c r="D106" s="16"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C107"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D103">
     <sortCondition ref="A82"/>

</xml_diff>

<commit_message>
Weekly Contest 206 (Problem 1582, 1583, 1584 & 1585)
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1581CD-862B-4C75-8AE1-34AD5509EBDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4039A1-9E05-47CC-ADB5-57B9D07A57EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="119">
   <si>
     <t>Name</t>
   </si>
@@ -370,6 +370,18 @@
   </si>
   <si>
     <t>Lowest Common Ancestor of a Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Special Positions in a Binary Matrix</t>
+  </si>
+  <si>
+    <t>Count Unhappy Friends</t>
+  </si>
+  <si>
+    <t>Min Cost to Connect All Points</t>
+  </si>
+  <si>
+    <t>Check If String Is Transformable With Substring Sort Operations</t>
   </si>
 </sst>
 </file>
@@ -973,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2107,6 +2119,46 @@
       <c r="C110" s="16"/>
       <c r="D110" s="16"/>
     </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="14">
+        <v>1582</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C111" s="15"/>
+      <c r="D111" s="15"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="14">
+        <v>1583</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C112" s="16"/>
+      <c r="D112" s="16"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="14">
+        <v>1584</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C113" s="16"/>
+      <c r="D113" s="16"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="14">
+        <v>1585</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C114" s="17"/>
+      <c r="D114" s="17"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D110">
     <sortCondition ref="A91"/>

</xml_diff>

<commit_message>
Problem 198, 213 & 1293
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF605B3-A6AF-4FD4-8B2A-B15F8703C812}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298C494A-5AAF-4231-8806-177B3F3D5F2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
   <si>
     <t>Name</t>
   </si>
@@ -385,6 +385,15 @@
   </si>
   <si>
     <t>Minimum Swaps to Group All 1's Together 🔒</t>
+  </si>
+  <si>
+    <t>House Robber</t>
+  </si>
+  <si>
+    <t>Shortest Path in a Grid with Obstacles Elimination</t>
+  </si>
+  <si>
+    <t>House Robber II</t>
   </si>
 </sst>
 </file>
@@ -988,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2172,6 +2181,36 @@
       <c r="C115" s="17"/>
       <c r="D115" s="17"/>
     </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="14">
+        <v>1293</v>
+      </c>
+      <c r="B116" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C116" s="17"/>
+      <c r="D116" s="17"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="14">
+        <v>198</v>
+      </c>
+      <c r="B117" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C117" s="15"/>
+      <c r="D117" s="16"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="14">
+        <v>213</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C118" s="16"/>
+      <c r="D118" s="16"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D115">
     <sortCondition ref="A94"/>

</xml_diff>

<commit_message>
Problem 329, 337 & 366
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298C494A-5AAF-4231-8806-177B3F3D5F2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD5DE7B-DD8E-4CAE-8D48-10C758BCDA36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="126">
   <si>
     <t>Name</t>
   </si>
@@ -394,6 +394,15 @@
   </si>
   <si>
     <t>House Robber II</t>
+  </si>
+  <si>
+    <t>Longest Increasing Path in a Matrix</t>
+  </si>
+  <si>
+    <t>House Robber III</t>
+  </si>
+  <si>
+    <t>Find Leaves of Binary Tree 🔒</t>
   </si>
 </sst>
 </file>
@@ -677,7 +686,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -997,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J118"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1763,457 +1772,487 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="14">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C74" s="16"/>
-      <c r="D74" s="15"/>
+        <v>120</v>
+      </c>
+      <c r="C74" s="15"/>
+      <c r="D74" s="16"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="14">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C75" s="15"/>
+        <v>97</v>
+      </c>
+      <c r="C75" s="16"/>
       <c r="D75" s="15"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="14">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="C76" s="16"/>
-      <c r="D76" s="16"/>
+        <v>36</v>
+      </c>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="14">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="C77" s="16"/>
       <c r="D77" s="16"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="14">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C78" s="15"/>
-      <c r="D78" s="15"/>
+        <v>122</v>
+      </c>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="14">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C79" s="21"/>
+        <v>37</v>
+      </c>
+      <c r="C79" s="16"/>
       <c r="D79" s="16"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="14">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="14">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C81" s="16"/>
+        <v>38</v>
+      </c>
+      <c r="C81" s="21"/>
       <c r="D81" s="16"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="14">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C82" s="16"/>
-      <c r="D82" s="17"/>
+        <v>111</v>
+      </c>
+      <c r="C82" s="15"/>
+      <c r="D82" s="15"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="14">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C83" s="16"/>
       <c r="D83" s="16"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="14">
-        <v>286</v>
+        <v>238</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>117</v>
+        <v>39</v>
       </c>
       <c r="C84" s="16"/>
-      <c r="D84" s="16"/>
+      <c r="D84" s="17"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="14">
-        <v>295</v>
+        <v>253</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C85" s="17"/>
-      <c r="D85" s="17"/>
+        <v>118</v>
+      </c>
+      <c r="C85" s="16"/>
+      <c r="D85" s="16"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="14">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="C86" s="16"/>
-      <c r="D86" s="17"/>
+      <c r="D86" s="16"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="14">
-        <v>322</v>
+        <v>295</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C87" s="16"/>
+        <v>100</v>
+      </c>
+      <c r="C87" s="17"/>
       <c r="D87" s="17"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="14">
-        <v>373</v>
+        <v>300</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C88" s="23"/>
       <c r="D88" s="17"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="14">
-        <v>394</v>
+        <v>322</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C89" s="16"/>
-      <c r="D89" s="16"/>
+      <c r="D89" s="17"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="14">
-        <v>509</v>
+        <v>329</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C90" s="15"/>
-      <c r="D90" s="15"/>
+        <v>123</v>
+      </c>
+      <c r="C90" s="17"/>
+      <c r="D90" s="16"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="14">
-        <v>518</v>
+        <v>337</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="C91" s="16"/>
       <c r="D91" s="16"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="14">
-        <v>647</v>
+        <v>366</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="C92" s="16"/>
       <c r="D92" s="16"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="14">
-        <v>990</v>
+        <v>373</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C93" s="22"/>
+        <v>42</v>
+      </c>
+      <c r="C93" s="16"/>
       <c r="D93" s="17"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="14">
-        <v>1143</v>
+        <v>394</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="C94" s="16"/>
-      <c r="D94" s="15"/>
+      <c r="D94" s="16"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="14">
-        <v>1151</v>
+        <v>509</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="C95" s="16"/>
-      <c r="D95" s="16"/>
+        <v>109</v>
+      </c>
+      <c r="C95" s="15"/>
+      <c r="D95" s="15"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="14">
-        <v>1439</v>
+        <v>518</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="C96" s="17"/>
-      <c r="D96" s="17"/>
+        <v>98</v>
+      </c>
+      <c r="C96" s="16"/>
+      <c r="D96" s="16"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="14">
-        <v>1550</v>
+        <v>647</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C97" s="15"/>
-      <c r="D97" s="15"/>
+        <v>44</v>
+      </c>
+      <c r="C97" s="16"/>
+      <c r="D97" s="16"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="14">
-        <v>1551</v>
+        <v>990</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C98" s="16"/>
-      <c r="D98" s="15"/>
+        <v>108</v>
+      </c>
+      <c r="C98" s="22"/>
+      <c r="D98" s="17"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="14">
-        <v>1552</v>
+        <v>1143</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C99" s="16"/>
-      <c r="D99" s="17"/>
+      <c r="D99" s="15"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="14">
-        <v>1553</v>
+        <v>1151</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C100" s="17"/>
+        <v>119</v>
+      </c>
+      <c r="C100" s="16"/>
       <c r="D100" s="16"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="14">
-        <v>1556</v>
+        <v>1293</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C101" s="15"/>
-      <c r="D101" s="15"/>
+        <v>121</v>
+      </c>
+      <c r="C101" s="17"/>
+      <c r="D101" s="17"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="14">
-        <v>1557</v>
+        <v>1439</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C102" s="16"/>
-      <c r="D102" s="16"/>
+        <v>116</v>
+      </c>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="14">
-        <v>1558</v>
+        <v>1550</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C103" s="16"/>
-      <c r="D103" s="17"/>
+        <v>63</v>
+      </c>
+      <c r="C103" s="15"/>
+      <c r="D103" s="15"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="14">
-        <v>1566</v>
+        <v>1551</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C104" s="15"/>
-      <c r="D104" s="16"/>
+        <v>64</v>
+      </c>
+      <c r="C104" s="16"/>
+      <c r="D104" s="15"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="14">
-        <v>1572</v>
+        <v>1552</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C105" s="15"/>
-      <c r="D105" s="15"/>
+        <v>65</v>
+      </c>
+      <c r="C105" s="16"/>
+      <c r="D105" s="17"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="14">
-        <v>1573</v>
+        <v>1553</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C106" s="16"/>
+        <v>66</v>
+      </c>
+      <c r="C106" s="17"/>
       <c r="D106" s="16"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="14">
-        <v>1574</v>
+        <v>1556</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="C107" s="24"/>
-      <c r="D107" s="17"/>
+      <c r="D107" s="15"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="14">
-        <v>1575</v>
+        <v>1557</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C108" s="17"/>
-      <c r="D108" s="17"/>
+        <v>81</v>
+      </c>
+      <c r="C108" s="16"/>
+      <c r="D108" s="16"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="14">
-        <v>1576</v>
+        <v>1558</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C109" s="15"/>
-      <c r="D109" s="16"/>
+        <v>82</v>
+      </c>
+      <c r="C109" s="16"/>
+      <c r="D109" s="17"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="14">
-        <v>1577</v>
+        <v>1566</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C110" s="16"/>
+        <v>91</v>
+      </c>
+      <c r="C110" s="15"/>
       <c r="D110" s="16"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="14">
-        <v>1578</v>
+        <v>1572</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C111" s="16"/>
-      <c r="D111" s="16"/>
+        <v>101</v>
+      </c>
+      <c r="C111" s="15"/>
+      <c r="D111" s="15"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="14">
-        <v>1582</v>
+        <v>1573</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C112" s="15"/>
-      <c r="D112" s="15"/>
+        <v>102</v>
+      </c>
+      <c r="C112" s="16"/>
+      <c r="D112" s="16"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="14">
-        <v>1583</v>
+        <v>1574</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C113" s="16"/>
-      <c r="D113" s="16"/>
+      <c r="D113" s="17"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="14">
-        <v>1584</v>
+        <v>1575</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C114" s="16"/>
-      <c r="D114" s="16"/>
+        <v>104</v>
+      </c>
+      <c r="C114" s="17"/>
+      <c r="D114" s="17"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="14">
-        <v>1585</v>
+        <v>1576</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C115" s="17"/>
-      <c r="D115" s="17"/>
+        <v>105</v>
+      </c>
+      <c r="C115" s="15"/>
+      <c r="D115" s="16"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="14">
-        <v>1293</v>
+        <v>1577</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C116" s="17"/>
-      <c r="D116" s="17"/>
+        <v>106</v>
+      </c>
+      <c r="C116" s="16"/>
+      <c r="D116" s="16"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="14">
-        <v>198</v>
+        <v>1578</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="C117" s="15"/>
+        <v>107</v>
+      </c>
+      <c r="C117" s="16"/>
       <c r="D117" s="16"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="14">
-        <v>213</v>
+        <v>1582</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="C118" s="16"/>
-      <c r="D118" s="16"/>
+        <v>112</v>
+      </c>
+      <c r="C118" s="15"/>
+      <c r="D118" s="15"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="14">
+        <v>1583</v>
+      </c>
+      <c r="B119" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C119" s="16"/>
+      <c r="D119" s="16"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="14">
+        <v>1584</v>
+      </c>
+      <c r="B120" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C120" s="16"/>
+      <c r="D120" s="16"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="14">
+        <v>1585</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C121" s="17"/>
+      <c r="D121" s="17"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D115">
-    <sortCondition ref="A94"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D121">
+    <sortCondition ref="A113"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Problem 84 & 863
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA\Coding\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993F1E7A-E197-4BF5-8A74-1E8A76B7F5AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C705E0-FC18-4594-9FC9-650076753CCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD1B1F98-D37A-49CF-8BD5-80A2CE994BC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="129">
   <si>
     <t>Name</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Product of Array Except Self</t>
   </si>
   <si>
-    <t>Longest Increasing Substring</t>
-  </si>
-  <si>
     <t>Coin Change</t>
   </si>
   <si>
@@ -406,6 +403,15 @@
   </si>
   <si>
     <t>Minimum Path Sum</t>
+  </si>
+  <si>
+    <t>Largest Rectangle in Histogram</t>
+  </si>
+  <si>
+    <t>Longest Increasing Subsequence</t>
+  </si>
+  <si>
+    <t>All Nodes Distance K in Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -686,10 +692,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1009,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134F0A3-D7E3-4AF7-B9B4-7756C1798D0F}">
-  <dimension ref="A1:J122"/>
+  <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1108,7 +1114,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="17"/>
@@ -1128,7 +1134,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
@@ -1148,7 +1154,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
@@ -1158,7 +1164,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -1198,7 +1204,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -1208,7 +1214,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="15"/>
@@ -1218,7 +1224,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -1228,7 +1234,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="15"/>
@@ -1258,7 +1264,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -1268,7 +1274,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
@@ -1308,7 +1314,7 @@
         <v>29</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="17"/>
@@ -1318,7 +1324,7 @@
         <v>31</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="16"/>
       <c r="D28" s="17"/>
@@ -1328,7 +1334,7 @@
         <v>33</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
@@ -1358,7 +1364,7 @@
         <v>36</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -1378,7 +1384,7 @@
         <v>39</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34" s="16"/>
       <c r="D34" s="17"/>
@@ -1388,7 +1394,7 @@
         <v>40</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C35" s="16"/>
       <c r="D35" s="17"/>
@@ -1398,7 +1404,7 @@
         <v>42</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C36" s="17"/>
       <c r="D36" s="16"/>
@@ -1408,7 +1414,7 @@
         <v>43</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C37" s="16"/>
       <c r="D37" s="17"/>
@@ -1418,7 +1424,7 @@
         <v>46</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C38" s="16"/>
       <c r="D38" s="15"/>
@@ -1428,7 +1434,7 @@
         <v>47</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39" s="16"/>
       <c r="D39" s="15"/>
@@ -1438,7 +1444,7 @@
         <v>48</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="15"/>
@@ -1448,7 +1454,7 @@
         <v>49</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C41" s="16"/>
       <c r="D41" s="15"/>
@@ -1458,7 +1464,7 @@
         <v>51</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
@@ -1488,7 +1494,7 @@
         <v>64</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C45" s="16"/>
       <c r="D45" s="15"/>
@@ -1538,7 +1544,7 @@
         <v>72</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C50" s="19"/>
       <c r="D50" s="17"/>
@@ -1548,7 +1554,7 @@
         <v>78</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -1565,347 +1571,347 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="14">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53" s="15"/>
+        <v>126</v>
+      </c>
+      <c r="C53" s="17"/>
       <c r="D53" s="16"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="16"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="14">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
+      <c r="D55" s="16"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="14">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C56" s="15"/>
       <c r="D56" s="15"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="14">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C57" s="15"/>
-      <c r="D57" s="16"/>
+      <c r="D57" s="15"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="14">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
+      <c r="D58" s="16"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="14">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C59" s="15"/>
-      <c r="D59" s="16"/>
+      <c r="D59" s="15"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="14">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
+      <c r="D60" s="16"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="14">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="14">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C62" s="15"/>
-      <c r="D62" s="16"/>
+      <c r="D62" s="15"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="14">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="16"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="14">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
+      <c r="D64" s="16"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="14">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="14">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C67" s="15"/>
       <c r="D67" s="15"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C68" s="15"/>
       <c r="D68" s="15"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="14">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C69" s="16"/>
-      <c r="D69" s="16"/>
+        <v>74</v>
+      </c>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="14">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
+        <v>34</v>
+      </c>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="14">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="C71" s="20"/>
-      <c r="D71" s="16"/>
+      <c r="D71" s="15"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="14">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
+      <c r="D72" s="16"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="14">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C73" s="20"/>
-      <c r="D73" s="16"/>
+      <c r="D73" s="15"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="14">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
+      <c r="D74" s="16"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="14">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="C75" s="15"/>
-      <c r="D75" s="16"/>
+      <c r="D75" s="15"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="14">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C76" s="16"/>
-      <c r="D76" s="15"/>
+        <v>119</v>
+      </c>
+      <c r="C76" s="15"/>
+      <c r="D76" s="16"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="14">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C77" s="15"/>
+        <v>96</v>
+      </c>
+      <c r="C77" s="16"/>
       <c r="D77" s="15"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="14">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="C78" s="16"/>
-      <c r="D78" s="16"/>
+        <v>36</v>
+      </c>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="14">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="C79" s="16"/>
       <c r="D79" s="16"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="14">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
       <c r="C80" s="16"/>
       <c r="D80" s="16"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="14">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
+        <v>37</v>
+      </c>
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="14">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C82" s="21"/>
-      <c r="D82" s="16"/>
+        <v>95</v>
+      </c>
+      <c r="C82" s="15"/>
+      <c r="D82" s="15"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="14">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="C83" s="15"/>
-      <c r="D83" s="15"/>
+        <v>38</v>
+      </c>
+      <c r="C83" s="21"/>
+      <c r="D83" s="16"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="14">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B84" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C84" s="16"/>
-      <c r="D84" s="16"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="15"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="14">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="C85" s="16"/>
-      <c r="D85" s="17"/>
+      <c r="D85" s="16"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="14">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="C86" s="16"/>
-      <c r="D86" s="16"/>
+      <c r="D86" s="17"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="14">
-        <v>286</v>
+        <v>253</v>
       </c>
       <c r="B87" s="14" t="s">
         <v>117</v>
@@ -1915,357 +1921,377 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="14">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="C88" s="24"/>
-      <c r="D88" s="17"/>
+      <c r="D88" s="16"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="14">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C89" s="16"/>
+        <v>99</v>
+      </c>
+      <c r="C89" s="17"/>
       <c r="D89" s="17"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="14">
-        <v>322</v>
+        <v>300</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="C90" s="16"/>
       <c r="D90" s="17"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="14">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="C91" s="17"/>
-      <c r="D91" s="16"/>
+        <v>40</v>
+      </c>
+      <c r="C91" s="16"/>
+      <c r="D91" s="17"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="14">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C92" s="16"/>
+        <v>122</v>
+      </c>
+      <c r="C92" s="17"/>
       <c r="D92" s="16"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="14">
-        <v>366</v>
+        <v>337</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C93" s="16"/>
       <c r="D93" s="16"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="14">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>42</v>
+        <v>124</v>
       </c>
       <c r="C94" s="16"/>
-      <c r="D94" s="17"/>
+      <c r="D94" s="16"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="14">
-        <v>394</v>
+        <v>373</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C95" s="16"/>
-      <c r="D95" s="16"/>
+      <c r="D95" s="17"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="14">
-        <v>509</v>
+        <v>394</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C96" s="15"/>
-      <c r="D96" s="15"/>
+        <v>42</v>
+      </c>
+      <c r="C96" s="16"/>
+      <c r="D96" s="16"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="14">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C97" s="16"/>
-      <c r="D97" s="16"/>
+        <v>108</v>
+      </c>
+      <c r="C97" s="15"/>
+      <c r="D97" s="15"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="14">
-        <v>647</v>
+        <v>518</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="C98" s="16"/>
       <c r="D98" s="16"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="14">
-        <v>990</v>
+        <v>647</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C99" s="22"/>
-      <c r="D99" s="17"/>
+        <v>43</v>
+      </c>
+      <c r="C99" s="16"/>
+      <c r="D99" s="16"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="14">
-        <v>1143</v>
+        <v>863</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="C100" s="16"/>
-      <c r="D100" s="15"/>
+      <c r="D100" s="16"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="14">
-        <v>1151</v>
+        <v>990</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="C101" s="16"/>
-      <c r="D101" s="16"/>
+        <v>107</v>
+      </c>
+      <c r="C101" s="22"/>
+      <c r="D101" s="17"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="14">
-        <v>1293</v>
+        <v>1143</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C102" s="17"/>
-      <c r="D102" s="17"/>
+        <v>93</v>
+      </c>
+      <c r="C102" s="16"/>
+      <c r="D102" s="15"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="14">
-        <v>1439</v>
+        <v>1151</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="C103" s="17"/>
-      <c r="D103" s="17"/>
+        <v>118</v>
+      </c>
+      <c r="C103" s="16"/>
+      <c r="D103" s="16"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="14">
-        <v>1550</v>
+        <v>1293</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C104" s="15"/>
-      <c r="D104" s="15"/>
+        <v>120</v>
+      </c>
+      <c r="C104" s="17"/>
+      <c r="D104" s="17"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="14">
-        <v>1551</v>
+        <v>1439</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C105" s="16"/>
-      <c r="D105" s="15"/>
+        <v>115</v>
+      </c>
+      <c r="C105" s="17"/>
+      <c r="D105" s="17"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="14">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C106" s="16"/>
-      <c r="D106" s="17"/>
+        <v>62</v>
+      </c>
+      <c r="C106" s="15"/>
+      <c r="D106" s="15"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="14">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C107" s="23"/>
-      <c r="D107" s="16"/>
+      <c r="D107" s="15"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="14">
-        <v>1556</v>
+        <v>1552</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C108" s="15"/>
-      <c r="D108" s="15"/>
+        <v>64</v>
+      </c>
+      <c r="C108" s="16"/>
+      <c r="D108" s="17"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="14">
-        <v>1557</v>
+        <v>1553</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C109" s="16"/>
+        <v>65</v>
+      </c>
+      <c r="C109" s="17"/>
       <c r="D109" s="16"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="14">
-        <v>1558</v>
+        <v>1556</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C110" s="16"/>
-      <c r="D110" s="17"/>
+        <v>79</v>
+      </c>
+      <c r="C110" s="15"/>
+      <c r="D110" s="15"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="14">
-        <v>1566</v>
+        <v>1557</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C111" s="15"/>
+        <v>80</v>
+      </c>
+      <c r="C111" s="16"/>
       <c r="D111" s="16"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="14">
-        <v>1572</v>
+        <v>1558</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C112" s="15"/>
-      <c r="D112" s="15"/>
+        <v>81</v>
+      </c>
+      <c r="C112" s="16"/>
+      <c r="D112" s="17"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="14">
-        <v>1573</v>
+        <v>1566</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C113" s="16"/>
+        <v>90</v>
+      </c>
+      <c r="C113" s="15"/>
       <c r="D113" s="16"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="14">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C114" s="16"/>
-      <c r="D114" s="17"/>
+        <v>100</v>
+      </c>
+      <c r="C114" s="15"/>
+      <c r="D114" s="15"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="14">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C115" s="17"/>
-      <c r="D115" s="17"/>
+        <v>101</v>
+      </c>
+      <c r="C115" s="16"/>
+      <c r="D115" s="16"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="14">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C116" s="15"/>
-      <c r="D116" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="C116" s="16"/>
+      <c r="D116" s="17"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="14">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C117" s="16"/>
-      <c r="D117" s="16"/>
+        <v>103</v>
+      </c>
+      <c r="C117" s="17"/>
+      <c r="D117" s="17"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="14">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C118" s="16"/>
+        <v>104</v>
+      </c>
+      <c r="C118" s="15"/>
       <c r="D118" s="16"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="14">
-        <v>1582</v>
+        <v>1577</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C119" s="15"/>
-      <c r="D119" s="15"/>
+        <v>105</v>
+      </c>
+      <c r="C119" s="16"/>
+      <c r="D119" s="16"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="14">
-        <v>1583</v>
+        <v>1578</v>
       </c>
       <c r="B120" s="14" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C120" s="16"/>
       <c r="D120" s="16"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="14">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C121" s="16"/>
-      <c r="D121" s="16"/>
+        <v>111</v>
+      </c>
+      <c r="C121" s="15"/>
+      <c r="D121" s="15"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="14">
+        <v>1583</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C122" s="16"/>
+      <c r="D122" s="16"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="14">
+        <v>1584</v>
+      </c>
+      <c r="B123" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C123" s="16"/>
+      <c r="D123" s="16"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="14">
         <v>1585</v>
       </c>
-      <c r="B122" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C122" s="17"/>
-      <c r="D122" s="17"/>
+      <c r="B124" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C124" s="17"/>
+      <c r="D124" s="17"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D122">
-    <sortCondition ref="A113"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D124">
+    <sortCondition ref="A104"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>